<commit_message>
Sort of got different-sku packing
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\source\repos\Bundle_Optimization\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C684E760-E992-4134-9106-225404A90503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5676A1C5-2920-4483-8D6A-88362D3F62A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="4" r:id="rId1"/>
@@ -972,13 +972,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1152,9 +1152,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1192,9 +1192,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1227,9 +1227,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,9 +1279,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1440,25 +1474,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4826BC9-1387-4C38-A76C-7A9E8593B627}">
   <dimension ref="A1:G267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="8"/>
@@ -1466,7 +1500,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1523,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1512,7 +1546,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1567,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1556,7 +1590,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1603,7 @@
         <v>76.199999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1582,7 +1616,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1595,7 +1629,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1644,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1623,7 +1657,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1646,7 +1680,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1667,7 +1701,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1722,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1745,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1732,7 +1766,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1753,7 +1787,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1776,7 +1810,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1797,7 +1831,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1810,7 +1844,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1823,7 +1857,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +1880,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +1901,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1924,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1911,7 +1945,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1924,7 +1958,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1937,7 +1971,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +1984,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1973,7 +2007,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -1994,7 +2028,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -2015,7 +2049,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -2038,7 +2072,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2051,7 +2085,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2074,7 +2108,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2087,7 +2121,7 @@
         <v>76.199999999999989</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2108,7 +2142,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2131,7 +2165,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2154,7 +2188,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -2175,7 +2209,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2198,7 +2232,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2221,7 +2255,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2242,7 +2276,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2265,7 +2299,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -2286,7 +2320,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -2299,7 +2333,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -2312,7 +2346,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -2335,7 +2369,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2356,7 +2390,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -2371,7 +2405,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2394,7 +2428,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -2415,7 +2449,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -2436,7 +2470,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -2459,7 +2493,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -2480,7 +2514,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -2503,7 +2537,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -2524,7 +2558,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -2545,7 +2579,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -2558,7 +2592,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -2581,7 +2615,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -2602,7 +2636,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -2623,7 +2657,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -2644,7 +2678,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -2665,7 +2699,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -2686,7 +2720,7 @@
         <v>177.8</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -2707,7 +2741,7 @@
         <v>203.2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -2728,7 +2762,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -2749,7 +2783,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -2770,7 +2804,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -2791,7 +2825,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -2804,7 +2838,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -2817,7 +2851,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -2830,7 +2864,7 @@
         <v>203.2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -2851,7 +2885,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -2872,7 +2906,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -2893,7 +2927,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -2914,7 +2948,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -2937,7 +2971,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -2958,7 +2992,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -2973,7 +3007,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -2986,7 +3020,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -3009,7 +3043,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -3030,7 +3064,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -3051,7 +3085,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -3074,7 +3108,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -3095,7 +3129,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -3110,7 +3144,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -3123,7 +3157,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -3136,7 +3170,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -3149,7 +3183,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -3172,7 +3206,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -3193,7 +3227,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -3216,7 +3250,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -3237,7 +3271,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -3260,7 +3294,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -3283,7 +3317,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -3304,7 +3338,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -3317,7 +3351,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -3338,7 +3372,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -3361,7 +3395,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -3384,7 +3418,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -3405,7 +3439,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
@@ -3420,7 +3454,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
@@ -3435,7 +3469,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
@@ -3450,7 +3484,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
@@ -3463,7 +3497,7 @@
         <v>76.199999999999989</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
@@ -3478,7 +3512,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -3501,7 +3535,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -3524,7 +3558,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
@@ -3545,7 +3579,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -3568,7 +3602,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -3591,7 +3625,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
@@ -3612,7 +3646,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
@@ -3627,7 +3661,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
@@ -3642,7 +3676,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
@@ -3657,7 +3691,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
@@ -3670,7 +3704,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -3693,7 +3727,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -3716,7 +3750,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
@@ -3737,7 +3771,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
@@ -3760,7 +3794,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
@@ -3783,7 +3817,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
@@ -3804,7 +3838,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
@@ -3827,7 +3861,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
@@ -3850,7 +3884,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
@@ -3871,7 +3905,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
@@ -3894,7 +3928,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
@@ -3917,7 +3951,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
@@ -3932,7 +3966,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
@@ -3945,7 +3979,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
@@ -3958,7 +3992,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
@@ -3971,7 +4005,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -3994,7 +4028,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
@@ -4015,7 +4049,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -4028,7 +4062,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
@@ -4041,7 +4075,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
@@ -4064,7 +4098,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
@@ -4085,7 +4119,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
@@ -4100,7 +4134,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
@@ -4115,7 +4149,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
@@ -4128,7 +4162,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
@@ -4141,7 +4175,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
@@ -4154,7 +4188,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
@@ -4177,7 +4211,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
@@ -4200,7 +4234,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
@@ -4221,7 +4255,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
@@ -4244,7 +4278,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
@@ -4267,7 +4301,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
@@ -4288,7 +4322,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
@@ -4311,7 +4345,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
@@ -4334,7 +4368,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
@@ -4355,7 +4389,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
@@ -4370,7 +4404,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
@@ -4393,7 +4427,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
@@ -4416,7 +4450,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
@@ -4439,7 +4473,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
@@ -4462,7 +4496,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
@@ -4483,7 +4517,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
@@ -4498,7 +4532,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
@@ -4511,7 +4545,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
@@ -4532,7 +4566,7 @@
         <v>304.8</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
@@ -4555,7 +4589,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
@@ -4578,7 +4612,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
@@ -4599,7 +4633,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
@@ -4622,7 +4656,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
@@ -4645,7 +4679,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
@@ -4668,7 +4702,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
@@ -4691,7 +4725,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
@@ -4712,7 +4746,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
@@ -4727,7 +4761,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
@@ -4742,7 +4776,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
@@ -4755,7 +4789,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
@@ -4770,7 +4804,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
@@ -4793,7 +4827,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
@@ -4814,7 +4848,7 @@
         <v>6121.4</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
@@ -4837,7 +4871,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
@@ -4858,7 +4892,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -4881,7 +4915,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
@@ -4902,7 +4936,7 @@
         <v>6426.2</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -4925,7 +4959,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
@@ -4946,7 +4980,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
@@ -4969,7 +5003,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
@@ -4992,7 +5026,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
@@ -5015,7 +5049,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
@@ -5036,7 +5070,7 @@
         <v>4902.2</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
@@ -5057,7 +5091,7 @@
         <v>6426.2</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
@@ -5080,7 +5114,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
@@ -5101,7 +5135,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
@@ -5116,7 +5150,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
@@ -5131,7 +5165,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
@@ -5146,7 +5180,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
@@ -5169,7 +5203,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
@@ -5192,7 +5226,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
@@ -5213,7 +5247,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
@@ -5228,7 +5262,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
@@ -5249,7 +5283,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
@@ -5262,7 +5296,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
@@ -5273,7 +5307,7 @@
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
@@ -5284,7 +5318,7 @@
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
@@ -5297,7 +5331,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
@@ -5310,7 +5344,7 @@
         <v>304.8</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
@@ -5323,7 +5357,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
@@ -5336,7 +5370,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
@@ -5349,7 +5383,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -5362,7 +5396,7 @@
         <v>203.2</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -5377,7 +5411,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -5390,7 +5424,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
@@ -5401,13 +5435,13 @@
       <c r="F206" s="1"/>
       <c r="G206" s="1"/>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D207" s="1">
         <v>0.63492063492063489</v>
@@ -5422,13 +5456,13 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1">
-        <v>1500</v>
+        <v>1</v>
       </c>
       <c r="D208" s="1">
         <v>9.0702947845804989</v>
@@ -5443,7 +5477,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>211</v>
       </c>
@@ -5454,7 +5488,7 @@
       <c r="F209" s="1"/>
       <c r="G209" s="1"/>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>212</v>
       </c>
@@ -5465,7 +5499,7 @@
       <c r="F210" s="1"/>
       <c r="G210" s="1"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>213</v>
       </c>
@@ -5480,7 +5514,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>214</v>
       </c>
@@ -5501,7 +5535,7 @@
         <v>228.6</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>215</v>
       </c>
@@ -5514,7 +5548,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>216</v>
       </c>
@@ -5525,7 +5559,7 @@
       <c r="F214" s="1"/>
       <c r="G214" s="1"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>217</v>
       </c>
@@ -5536,7 +5570,7 @@
       <c r="F215" s="1"/>
       <c r="G215" s="1"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>266</v>
       </c>
@@ -5557,7 +5591,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>218</v>
       </c>
@@ -5568,7 +5602,7 @@
       <c r="F217" s="1"/>
       <c r="G217" s="1"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>265</v>
       </c>
@@ -5589,7 +5623,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>219</v>
       </c>
@@ -5600,7 +5634,7 @@
       <c r="F219" s="1"/>
       <c r="G219" s="1"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>220</v>
       </c>
@@ -5611,7 +5645,7 @@
       <c r="F220" s="1"/>
       <c r="G220" s="1"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>221</v>
       </c>
@@ -5622,7 +5656,7 @@
       <c r="F221" s="1"/>
       <c r="G221" s="1"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>222</v>
       </c>
@@ -5633,7 +5667,7 @@
       <c r="F222" s="1"/>
       <c r="G222" s="1"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>223</v>
       </c>
@@ -5644,7 +5678,7 @@
       <c r="F223" s="1"/>
       <c r="G223" s="1"/>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>224</v>
       </c>
@@ -5667,7 +5701,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>225</v>
       </c>
@@ -5688,7 +5722,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>226</v>
       </c>
@@ -5709,7 +5743,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>227</v>
       </c>
@@ -5732,7 +5766,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>228</v>
       </c>
@@ -5753,7 +5787,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>229</v>
       </c>
@@ -5774,7 +5808,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>230</v>
       </c>
@@ -5795,7 +5829,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>231</v>
       </c>
@@ -5810,7 +5844,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>232</v>
       </c>
@@ -5823,7 +5857,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>233</v>
       </c>
@@ -5838,7 +5872,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>1</v>
       </c>
@@ -5849,7 +5883,7 @@
       <c r="F234" s="1"/>
       <c r="G234" s="1"/>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
@@ -5860,7 +5894,7 @@
       <c r="F235" s="1"/>
       <c r="G235" s="1"/>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
@@ -5871,7 +5905,7 @@
       <c r="F236" s="1"/>
       <c r="G236" s="1"/>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
@@ -5882,7 +5916,7 @@
       <c r="F237" s="1"/>
       <c r="G237" s="1"/>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
@@ -5893,7 +5927,7 @@
       <c r="F238" s="1"/>
       <c r="G238" s="1"/>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
@@ -5904,7 +5938,7 @@
       <c r="F239" s="1"/>
       <c r="G239" s="1"/>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>2</v>
       </c>
@@ -5915,7 +5949,7 @@
       <c r="F240" s="1"/>
       <c r="G240" s="1"/>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
@@ -5926,7 +5960,7 @@
       <c r="F241" s="1"/>
       <c r="G241" s="1"/>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -5945,7 +5979,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
@@ -5958,7 +5992,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
@@ -5979,7 +6013,7 @@
         <v>355.6</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
@@ -5994,7 +6028,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
@@ -6009,7 +6043,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
@@ -6024,7 +6058,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
@@ -6039,7 +6073,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
@@ -6054,7 +6088,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
@@ -6069,7 +6103,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
@@ -6084,7 +6118,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
@@ -6099,7 +6133,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
@@ -6114,7 +6148,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
@@ -6129,7 +6163,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
@@ -6144,7 +6178,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
@@ -6159,7 +6193,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
@@ -6174,7 +6208,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>256</v>
       </c>
@@ -6189,7 +6223,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
@@ -6204,7 +6238,7 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
@@ -6215,7 +6249,7 @@
       <c r="F260" s="1"/>
       <c r="G260" s="1"/>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>3</v>
       </c>
@@ -6236,7 +6270,7 @@
         <v>177.8</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>259</v>
       </c>
@@ -6247,7 +6281,7 @@
       <c r="F262" s="1"/>
       <c r="G262" s="1"/>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>260</v>
       </c>
@@ -6262,7 +6296,7 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>261</v>
       </c>
@@ -6273,7 +6307,7 @@
       <c r="F264" s="1"/>
       <c r="G264" s="1"/>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>262</v>
       </c>
@@ -6284,7 +6318,7 @@
       <c r="F265" s="1"/>
       <c r="G265" s="1"/>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>263</v>
       </c>
@@ -6295,7 +6329,7 @@
       <c r="F266" s="1"/>
       <c r="G266" s="1"/>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>264</v>
       </c>

</xml_diff>

<commit_message>
Added most changes from part 1
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\source\repos\Bundle_Optimization\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5676A1C5-2920-4483-8D6A-88362D3F62A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E1822B-2CE7-46A0-83B4-191547804063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="275">
   <si>
     <t>SKU</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>Bottom Row Acceptable</t>
+  </si>
+  <si>
+    <t>Partial Dim To Reduce</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
@@ -964,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -982,11 +988,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1136,25 +1160,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46BB815A-07E7-45FC-AB22-C43EDD8C1539}" name="Table1" displayName="Table1" ref="A2:G267" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G267" xr:uid="{46BB815A-07E7-45FC-AB22-C43EDD8C1539}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B99C9ADF-7B02-4688-BF2B-FA64FF263304}" name="SKU" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F4A92998-C5C8-4CAC-BB26-61E001357CE3}" name="Bottom Row Acceptable" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A32B8FC9-EFFA-499A-9A63-C08CD0048436}" name="Qty/bundle" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7EEF0A5F-0BB1-4616-A54A-63B11FF8C703}" name="Weight kg/length" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{83AF6A44-741C-4065-87D9-3C81144083E0}" name="Width (mm)" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2847031E-B872-4761-94D6-2EAD311FE922}" name="Height (mm)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{3AF3E323-4DAC-4D05-B7FD-3AEFC66BEC50}" name="Length (mm)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46BB815A-07E7-45FC-AB22-C43EDD8C1539}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A2:H1048576" xr:uid="{46BB815A-07E7-45FC-AB22-C43EDD8C1539}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B99C9ADF-7B02-4688-BF2B-FA64FF263304}" name="SKU" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F4A92998-C5C8-4CAC-BB26-61E001357CE3}" name="Bottom Row Acceptable" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A32B8FC9-EFFA-499A-9A63-C08CD0048436}" name="Qty/bundle" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7EEF0A5F-0BB1-4616-A54A-63B11FF8C703}" name="Weight kg/length" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{83AF6A44-741C-4065-87D9-3C81144083E0}" name="Width (mm)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{2847031E-B872-4761-94D6-2EAD311FE922}" name="Height (mm)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{3AF3E323-4DAC-4D05-B7FD-3AEFC66BEC50}" name="Length (mm)" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{881BDB16-8334-48A1-A932-8A06FE6F1F33}" name="Partial Dim To Reduce" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1192,9 +1217,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1227,26 +1252,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1279,26 +1287,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1472,24 +1463,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4826BC9-1387-4C38-A76C-7A9E8593B627}">
-  <dimension ref="A1:G267"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E210" sqref="E210"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="7" t="s">
@@ -1500,7 +1492,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1522,8 +1514,11 @@
       <c r="G2" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1545,12 +1540,14 @@
       <c r="G3" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>4</v>
       </c>
@@ -1566,8 +1563,11 @@
       <c r="G4" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1589,75 +1589,54 @@
       <c r="G5" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
       <c r="G6" s="1">
         <v>76.199999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
       <c r="G7" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
       <c r="G8" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>145</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
       <c r="G9" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1679,12 +1658,14 @@
       <c r="G11" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>4</v>
       </c>
@@ -1700,12 +1681,14 @@
       <c r="G12" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>4</v>
       </c>
@@ -1721,8 +1704,11 @@
       <c r="G13" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1744,12 +1730,14 @@
       <c r="G14" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -1765,12 +1753,14 @@
       <c r="G15" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>10</v>
       </c>
@@ -1786,8 +1776,11 @@
       <c r="G16" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1809,12 +1802,14 @@
       <c r="G17" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1"/>
       <c r="C18" s="1">
         <v>20</v>
       </c>
@@ -1830,34 +1825,27 @@
       <c r="G18" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
       <c r="G19" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
       <c r="G20" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1879,12 +1867,14 @@
       <c r="G21" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1"/>
       <c r="C22" s="1">
         <v>4</v>
       </c>
@@ -1900,8 +1890,11 @@
       <c r="G22" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1923,12 +1916,14 @@
       <c r="G23" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
       <c r="C24" s="1">
         <v>10</v>
       </c>
@@ -1944,47 +1939,35 @@
       <c r="G24" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
       <c r="G25" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
       <c r="G26" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
       <c r="G27" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2006,12 +1989,14 @@
       <c r="G28" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="1"/>
       <c r="C29" s="1">
         <v>20</v>
       </c>
@@ -2027,12 +2012,14 @@
       <c r="G29" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="1"/>
       <c r="C30" s="1">
         <v>20</v>
       </c>
@@ -2048,8 +2035,11 @@
       <c r="G30" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -2071,21 +2061,22 @@
       <c r="G31" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
       <c r="G32" s="1">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2107,25 +2098,25 @@
       <c r="G33" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
       <c r="G34" s="1">
         <v>76.199999999999989</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="1"/>
       <c r="C35" s="1">
         <v>10</v>
       </c>
@@ -2141,8 +2132,11 @@
       <c r="G35" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2164,8 +2158,11 @@
       <c r="G36" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2187,12 +2184,14 @@
       <c r="G37" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="1"/>
       <c r="C38" s="1">
         <v>4</v>
       </c>
@@ -2208,8 +2207,11 @@
       <c r="G38" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2231,8 +2233,11 @@
       <c r="G39" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2254,12 +2259,14 @@
       <c r="G40" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="1"/>
       <c r="C41" s="1">
         <v>4</v>
       </c>
@@ -2275,8 +2282,11 @@
       <c r="G41" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2298,12 +2308,14 @@
       <c r="G42" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="1"/>
       <c r="C43" s="1">
         <v>10</v>
       </c>
@@ -2319,34 +2331,27 @@
       <c r="G43" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
       <c r="G44" s="1">
         <v>101.6</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
       <c r="G45" s="1">
         <v>152.4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -2368,12 +2373,14 @@
       <c r="G46" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="1"/>
       <c r="C47" s="1">
         <v>10</v>
       </c>
@@ -2389,23 +2396,22 @@
       <c r="G47" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B48" s="1">
         <v>289</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
       <c r="G48" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2427,12 +2433,14 @@
       <c r="G49" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="1"/>
       <c r="C50" s="1">
         <v>4</v>
       </c>
@@ -2448,12 +2456,14 @@
       <c r="G50" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="1"/>
       <c r="C51" s="1">
         <v>4</v>
       </c>
@@ -2469,8 +2479,11 @@
       <c r="G51" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -2492,12 +2505,14 @@
       <c r="G52" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="1"/>
       <c r="C53" s="1">
         <v>8</v>
       </c>
@@ -2513,8 +2528,11 @@
       <c r="G53" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -2536,12 +2554,14 @@
       <c r="G54" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="1"/>
       <c r="C55" s="1">
         <v>4</v>
       </c>
@@ -2557,12 +2577,14 @@
       <c r="G55" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="1"/>
       <c r="C56" s="1">
         <v>4</v>
       </c>
@@ -2578,21 +2600,19 @@
       <c r="G56" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
       <c r="G57" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -2614,12 +2634,14 @@
       <c r="G58" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="1"/>
       <c r="C59" s="1">
         <v>10</v>
       </c>
@@ -2635,12 +2657,14 @@
       <c r="G59" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="1"/>
       <c r="C60" s="1">
         <v>20</v>
       </c>
@@ -2656,12 +2680,14 @@
       <c r="G60" s="1">
         <v>127</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="1"/>
       <c r="C61" s="1">
         <v>20</v>
       </c>
@@ -2677,12 +2703,14 @@
       <c r="G61" s="1">
         <v>152.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="1"/>
       <c r="C62" s="1">
         <v>20</v>
       </c>
@@ -2698,12 +2726,14 @@
       <c r="G62" s="1">
         <v>152.4</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="1"/>
       <c r="C63" s="1">
         <v>20</v>
       </c>
@@ -2719,12 +2749,14 @@
       <c r="G63" s="1">
         <v>177.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="1"/>
       <c r="C64" s="1">
         <v>20</v>
       </c>
@@ -2740,12 +2772,14 @@
       <c r="G64" s="1">
         <v>203.2</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="1"/>
       <c r="C65" s="1">
         <v>20</v>
       </c>
@@ -2761,12 +2795,14 @@
       <c r="G65" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="1"/>
       <c r="C66" s="1">
         <v>20</v>
       </c>
@@ -2782,12 +2818,14 @@
       <c r="G66" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="1"/>
       <c r="C67" s="1">
         <v>20</v>
       </c>
@@ -2803,12 +2841,14 @@
       <c r="G67" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="1"/>
       <c r="C68" s="1">
         <v>20</v>
       </c>
@@ -2824,51 +2864,38 @@
       <c r="G68" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
       <c r="G69" s="1">
         <v>101.6</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
       <c r="G70" s="1">
         <v>152.4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
       <c r="G71" s="1">
         <v>203.2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="1"/>
       <c r="C72" s="1">
         <v>20</v>
       </c>
@@ -2884,12 +2911,14 @@
       <c r="G72" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="1"/>
       <c r="C73" s="1">
         <v>20</v>
       </c>
@@ -2905,12 +2934,14 @@
       <c r="G73" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="1"/>
       <c r="C74" s="1">
         <v>20</v>
       </c>
@@ -2926,12 +2957,14 @@
       <c r="G74" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="1"/>
       <c r="C75" s="1">
         <v>20</v>
       </c>
@@ -2947,8 +2980,11 @@
       <c r="G75" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -2970,12 +3006,14 @@
       <c r="G76" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="1"/>
       <c r="C77" s="1">
         <v>10</v>
       </c>
@@ -2991,36 +3029,30 @@
       <c r="G77" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B78" s="1">
         <v>145</v>
       </c>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
       <c r="G78" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
       <c r="G79" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -3042,12 +3074,14 @@
       <c r="G80" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="1"/>
       <c r="C81" s="1">
         <v>20</v>
       </c>
@@ -3063,12 +3097,14 @@
       <c r="G81" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B82" s="1"/>
       <c r="C82" s="1">
         <v>20</v>
       </c>
@@ -3084,8 +3120,11 @@
       <c r="G82" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -3107,12 +3146,14 @@
       <c r="G83" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="1"/>
       <c r="C84" s="1">
         <v>10</v>
       </c>
@@ -3128,62 +3169,46 @@
       <c r="G84" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B85" s="1">
         <v>145</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
       <c r="G85" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
       <c r="G86" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
       <c r="G87" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
       <c r="G88" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -3205,12 +3230,14 @@
       <c r="G89" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B90" s="1"/>
       <c r="C90" s="1">
         <v>20</v>
       </c>
@@ -3226,8 +3253,11 @@
       <c r="G90" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -3249,12 +3279,14 @@
       <c r="G91" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B92" s="1"/>
       <c r="C92" s="1">
         <v>10</v>
       </c>
@@ -3270,8 +3302,11 @@
       <c r="G92" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -3293,8 +3328,11 @@
       <c r="G93" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -3316,12 +3354,14 @@
       <c r="G94" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="1"/>
       <c r="C95" s="1">
         <v>8</v>
       </c>
@@ -3337,25 +3377,22 @@
       <c r="G95" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
       <c r="G96" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B97" s="1"/>
       <c r="C97" s="1">
         <v>100</v>
       </c>
@@ -3371,8 +3408,11 @@
       <c r="G97" s="1">
         <v>381</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -3394,8 +3434,11 @@
       <c r="G98" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -3417,12 +3460,14 @@
       <c r="G99" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B100" s="1"/>
       <c r="C100" s="1">
         <v>4</v>
       </c>
@@ -3438,81 +3483,63 @@
       <c r="G100" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B101" s="1">
         <v>145</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
       <c r="G101" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B102" s="1">
         <v>289</v>
       </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
       <c r="G102" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B103" s="1">
         <v>289</v>
       </c>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
       <c r="G103" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
       <c r="G104" s="1">
         <v>76.199999999999989</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B105" s="1">
         <v>289</v>
       </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
       <c r="G105" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -3534,8 +3561,11 @@
       <c r="G106" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -3557,12 +3587,14 @@
       <c r="G107" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="1"/>
       <c r="C108" s="1">
         <v>4</v>
       </c>
@@ -3578,8 +3610,11 @@
       <c r="G108" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -3601,8 +3636,11 @@
       <c r="G109" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -3624,12 +3662,14 @@
       <c r="G110" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B111" s="1"/>
       <c r="C111" s="1">
         <v>4</v>
       </c>
@@ -3645,66 +3685,52 @@
       <c r="G111" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B112" s="1">
         <v>145</v>
       </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
       <c r="G112" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B113" s="1">
         <v>145</v>
       </c>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
       <c r="G113" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B114" s="1">
         <v>289</v>
       </c>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
       <c r="G114" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
       <c r="G115" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -3726,8 +3752,11 @@
       <c r="G116" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -3749,12 +3778,14 @@
       <c r="G117" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B118" s="1"/>
       <c r="C118" s="1">
         <v>4</v>
       </c>
@@ -3770,8 +3801,11 @@
       <c r="G118" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H118" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
@@ -3793,8 +3827,11 @@
       <c r="G119" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H119" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
@@ -3816,12 +3853,14 @@
       <c r="G120" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H120" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B121" s="1"/>
       <c r="C121" s="1">
         <v>4</v>
       </c>
@@ -3837,8 +3876,11 @@
       <c r="G121" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H121" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
@@ -3860,8 +3902,11 @@
       <c r="G122" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
@@ -3883,12 +3928,14 @@
       <c r="G123" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H123" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B124" s="1"/>
       <c r="C124" s="1">
         <v>2</v>
       </c>
@@ -3904,8 +3951,11 @@
       <c r="G124" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H124" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
@@ -3927,8 +3977,11 @@
       <c r="G125" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
@@ -3950,62 +4003,46 @@
       <c r="G126" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B127" s="1">
         <v>145</v>
       </c>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
       <c r="G127" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
       <c r="G128" s="1">
         <v>25.4</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
       <c r="G129" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
       <c r="G130" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -4027,12 +4064,14 @@
       <c r="G131" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B132" s="1"/>
       <c r="C132" s="1">
         <v>8</v>
       </c>
@@ -4048,34 +4087,33 @@
       <c r="G132" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
-      <c r="D133" s="1"/>
-      <c r="E133" s="1"/>
-      <c r="F133" s="1"/>
       <c r="G133" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
       <c r="G134" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H134" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
@@ -4097,12 +4135,14 @@
       <c r="G135" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H135" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B136" s="1"/>
       <c r="C136" s="1">
         <v>8</v>
       </c>
@@ -4118,77 +4158,57 @@
       <c r="G136" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H136" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B137" s="1">
         <v>145</v>
       </c>
-      <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
-      <c r="F137" s="1"/>
       <c r="G137" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B138" s="1">
         <v>289</v>
       </c>
-      <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
       <c r="G138" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
-      <c r="E139" s="1"/>
-      <c r="F139" s="1"/>
       <c r="G139" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
-      <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
       <c r="G140" s="1">
         <v>101.6</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
       <c r="G141" s="1">
         <v>152.4</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
@@ -4210,8 +4230,11 @@
       <c r="G142" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H142" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
@@ -4233,12 +4256,14 @@
       <c r="G143" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H143" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B144" s="1"/>
       <c r="C144" s="1">
         <v>12</v>
       </c>
@@ -4254,8 +4279,11 @@
       <c r="G144" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H144" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
@@ -4277,8 +4305,11 @@
       <c r="G145" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
@@ -4300,12 +4331,14 @@
       <c r="G146" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B147" s="1"/>
       <c r="C147" s="1">
         <v>2</v>
       </c>
@@ -4321,8 +4354,11 @@
       <c r="G147" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H147" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
@@ -4344,8 +4380,11 @@
       <c r="G148" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H148" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
@@ -4367,12 +4406,14 @@
       <c r="G149" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H149" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B150" s="1"/>
       <c r="C150" s="1">
         <v>2</v>
       </c>
@@ -4388,23 +4429,22 @@
       <c r="G150" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H150" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B151" s="1">
         <v>145</v>
       </c>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="F151" s="1"/>
       <c r="G151" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
@@ -4426,8 +4466,11 @@
       <c r="G152" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
@@ -4449,8 +4492,11 @@
       <c r="G153" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H153" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
@@ -4472,8 +4518,11 @@
       <c r="G154" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H154" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
@@ -4495,12 +4544,14 @@
       <c r="G155" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H155" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B156" s="1"/>
       <c r="C156" s="1">
         <v>8</v>
       </c>
@@ -4516,40 +4567,33 @@
       <c r="G156" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H156" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B157" s="1">
         <v>145</v>
       </c>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
       <c r="G157" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
       <c r="G158" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B159" s="1"/>
       <c r="C159" s="1">
         <v>25</v>
       </c>
@@ -4565,8 +4609,11 @@
       <c r="G159" s="1">
         <v>304.8</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H159" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
@@ -4588,8 +4635,11 @@
       <c r="G160" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H160" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
@@ -4611,12 +4661,14 @@
       <c r="G161" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H161" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B162" s="1"/>
       <c r="C162" s="1">
         <v>8</v>
       </c>
@@ -4632,8 +4684,11 @@
       <c r="G162" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H162" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
@@ -4655,8 +4710,11 @@
       <c r="G163" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H163" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
@@ -4678,8 +4736,11 @@
       <c r="G164" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H164" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
@@ -4701,8 +4762,11 @@
       <c r="G165" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H165" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
@@ -4724,12 +4788,14 @@
       <c r="G166" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H166" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B167" s="1"/>
       <c r="C167" s="1">
         <v>8</v>
       </c>
@@ -4745,66 +4811,52 @@
       <c r="G167" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H167" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B168" s="1">
         <v>145</v>
       </c>
-      <c r="C168" s="1"/>
-      <c r="D168" s="1"/>
-      <c r="E168" s="1"/>
-      <c r="F168" s="1"/>
       <c r="G168" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B169" s="1">
         <v>289</v>
       </c>
-      <c r="C169" s="1"/>
-      <c r="D169" s="1"/>
-      <c r="E169" s="1"/>
-      <c r="F169" s="1"/>
       <c r="G169" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
-      <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
-      <c r="F170" s="1"/>
       <c r="G170" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B171" s="1">
         <v>145</v>
       </c>
-      <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
       <c r="G171" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
@@ -4826,12 +4878,14 @@
       <c r="G172" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H172" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B173" s="1"/>
       <c r="C173" s="1">
         <v>8</v>
       </c>
@@ -4847,8 +4901,11 @@
       <c r="G173" s="1">
         <v>6121.4</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H173" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
@@ -4870,12 +4927,14 @@
       <c r="G174" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H174" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B175" s="1"/>
       <c r="C175" s="1">
         <v>8</v>
       </c>
@@ -4891,8 +4950,11 @@
       <c r="G175" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H175" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -4914,12 +4976,14 @@
       <c r="G176" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H176" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B177" s="1"/>
       <c r="C177" s="1">
         <v>8</v>
       </c>
@@ -4935,8 +4999,11 @@
       <c r="G177" s="1">
         <v>6426.2</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H177" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -4958,12 +5025,14 @@
       <c r="G178" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H178" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B179" s="1"/>
       <c r="C179" s="1">
         <v>8</v>
       </c>
@@ -4979,8 +5048,11 @@
       <c r="G179" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H179" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
@@ -5002,8 +5074,11 @@
       <c r="G180" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H180" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
@@ -5025,8 +5100,11 @@
       <c r="G181" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H181" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
@@ -5048,12 +5126,14 @@
       <c r="G182" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H182" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B183" s="1"/>
       <c r="C183" s="1">
         <v>8</v>
       </c>
@@ -5069,12 +5149,14 @@
       <c r="G183" s="1">
         <v>4902.2</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H183" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B184" s="1"/>
       <c r="C184" s="1">
         <v>8</v>
       </c>
@@ -5090,8 +5172,11 @@
       <c r="G184" s="1">
         <v>6426.2</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H184" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
@@ -5113,12 +5198,14 @@
       <c r="G185" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H185" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B186" s="1"/>
       <c r="C186" s="1">
         <v>8</v>
       </c>
@@ -5134,53 +5221,44 @@
       <c r="G186" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H186" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B187" s="1">
         <v>145</v>
       </c>
-      <c r="C187" s="1"/>
-      <c r="D187" s="1"/>
-      <c r="E187" s="1"/>
-      <c r="F187" s="1"/>
       <c r="G187" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B188" s="1">
         <v>145</v>
       </c>
-      <c r="C188" s="1"/>
-      <c r="D188" s="1"/>
-      <c r="E188" s="1"/>
-      <c r="F188" s="1"/>
       <c r="G188" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B189" s="1">
         <v>289</v>
       </c>
-      <c r="C189" s="1"/>
-      <c r="D189" s="1"/>
-      <c r="E189" s="1"/>
-      <c r="F189" s="1"/>
       <c r="G189" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
@@ -5202,8 +5280,11 @@
       <c r="G190" s="1">
         <v>3683</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H190" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
@@ -5225,12 +5306,14 @@
       <c r="G191" s="1">
         <v>7340.5999999999995</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H191" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B192" s="1"/>
       <c r="C192" s="1">
         <v>8</v>
       </c>
@@ -5246,27 +5329,25 @@
       <c r="G192" s="1">
         <v>1828.8</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H192" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B193" s="1">
         <v>145</v>
       </c>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1"/>
-      <c r="E193" s="1"/>
-      <c r="F193" s="1"/>
       <c r="G193" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B194" s="1"/>
       <c r="C194" s="1">
         <v>53</v>
       </c>
@@ -5282,164 +5363,104 @@
       <c r="G194" s="1">
         <v>127</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H194" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B195" s="1"/>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1"/>
-      <c r="E195" s="1"/>
-      <c r="F195" s="1"/>
       <c r="G195" s="1">
         <v>152.4</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B196" s="1"/>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1"/>
-      <c r="E196" s="1"/>
-      <c r="F196" s="1"/>
-      <c r="G196" s="1"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B197" s="1"/>
-      <c r="C197" s="1"/>
-      <c r="D197" s="1"/>
-      <c r="E197" s="1"/>
-      <c r="F197" s="1"/>
-      <c r="G197" s="1"/>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B198" s="1"/>
-      <c r="C198" s="1"/>
-      <c r="D198" s="1"/>
-      <c r="E198" s="1"/>
-      <c r="F198" s="1"/>
       <c r="G198" s="1">
         <v>254</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
-      <c r="D199" s="1"/>
-      <c r="E199" s="1"/>
-      <c r="F199" s="1"/>
       <c r="G199" s="1">
         <v>304.8</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1"/>
-      <c r="E200" s="1"/>
-      <c r="F200" s="1"/>
       <c r="G200" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B201" s="1"/>
-      <c r="C201" s="1"/>
-      <c r="D201" s="1"/>
-      <c r="E201" s="1"/>
-      <c r="F201" s="1"/>
       <c r="G201" s="1">
         <v>101.6</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
-      <c r="D202" s="1"/>
-      <c r="E202" s="1"/>
-      <c r="F202" s="1"/>
       <c r="G202" s="1">
         <v>152.4</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
-      <c r="D203" s="1"/>
-      <c r="E203" s="1"/>
-      <c r="F203" s="1"/>
       <c r="G203" s="1">
         <v>203.2</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B204" s="1">
         <v>289</v>
       </c>
-      <c r="C204" s="1"/>
-      <c r="D204" s="1"/>
-      <c r="E204" s="1"/>
-      <c r="F204" s="1"/>
       <c r="G204" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B205" s="1"/>
-      <c r="C205" s="1"/>
-      <c r="D205" s="1"/>
-      <c r="E205" s="1"/>
-      <c r="F205" s="1"/>
       <c r="G205" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1"/>
-      <c r="E206" s="1"/>
-      <c r="F206" s="1"/>
-      <c r="G206" s="1"/>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B207" s="1"/>
       <c r="C207" s="1">
         <v>1</v>
       </c>
@@ -5456,11 +5477,10 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B208" s="1"/>
       <c r="C208" s="1">
         <v>1</v>
       </c>
@@ -5477,48 +5497,31 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B209" s="1"/>
-      <c r="C209" s="1"/>
-      <c r="D209" s="1"/>
-      <c r="E209" s="1"/>
-      <c r="F209" s="1"/>
-      <c r="G209" s="1"/>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
-      <c r="G210" s="1"/>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B211" s="1">
         <v>289</v>
       </c>
-      <c r="C211" s="1"/>
-      <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
       <c r="G211" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B212" s="1"/>
       <c r="C212" s="1">
         <v>20</v>
       </c>
@@ -5535,46 +5538,28 @@
         <v>228.6</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B213" s="1"/>
-      <c r="C213" s="1"/>
-      <c r="D213" s="1"/>
-      <c r="E213" s="1"/>
-      <c r="F213" s="1"/>
       <c r="G213" s="1">
         <v>50.8</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
-      <c r="D214" s="1"/>
-      <c r="E214" s="1"/>
-      <c r="F214" s="1"/>
-      <c r="G214" s="1"/>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
-      <c r="D215" s="1"/>
-      <c r="E215" s="1"/>
-      <c r="F215" s="1"/>
-      <c r="G215" s="1"/>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B216" s="1"/>
       <c r="C216" s="1">
         <v>50</v>
       </c>
@@ -5591,22 +5576,15 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
-      <c r="F217" s="1"/>
-      <c r="G217" s="1"/>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B218" s="1"/>
       <c r="C218" s="1">
         <v>1</v>
       </c>
@@ -5623,62 +5601,32 @@
         <v>508</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
-      <c r="D219" s="1"/>
-      <c r="E219" s="1"/>
-      <c r="F219" s="1"/>
-      <c r="G219" s="1"/>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
-      <c r="D220" s="1"/>
-      <c r="E220" s="1"/>
-      <c r="F220" s="1"/>
-      <c r="G220" s="1"/>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B221" s="1"/>
-      <c r="C221" s="1"/>
-      <c r="D221" s="1"/>
-      <c r="E221" s="1"/>
-      <c r="F221" s="1"/>
-      <c r="G221" s="1"/>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1"/>
-      <c r="E222" s="1"/>
-      <c r="F222" s="1"/>
-      <c r="G222" s="1"/>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
-      <c r="G223" s="1"/>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>224</v>
       </c>
@@ -5701,11 +5649,10 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B225" s="1"/>
       <c r="C225" s="1">
         <v>10</v>
       </c>
@@ -5722,11 +5669,10 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B226" s="1"/>
       <c r="C226" s="1">
         <v>10</v>
       </c>
@@ -5743,7 +5689,7 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>227</v>
       </c>
@@ -5766,11 +5712,10 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B228" s="1"/>
       <c r="C228" s="1">
         <v>20</v>
       </c>
@@ -5787,11 +5732,10 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B229" s="1"/>
       <c r="C229" s="1">
         <v>20</v>
       </c>
@@ -5808,11 +5752,10 @@
         <v>1828.8</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B230" s="1"/>
       <c r="C230" s="1">
         <v>10</v>
       </c>
@@ -5829,138 +5772,77 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B231" s="1">
         <v>145</v>
       </c>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="1"/>
-      <c r="F231" s="1"/>
       <c r="G231" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
-      <c r="D232" s="1"/>
-      <c r="E232" s="1"/>
-      <c r="F232" s="1"/>
       <c r="G232" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>233</v>
       </c>
       <c r="B233" s="1">
         <v>289</v>
       </c>
-      <c r="C233" s="1"/>
-      <c r="D233" s="1"/>
-      <c r="E233" s="1"/>
-      <c r="F233" s="1"/>
       <c r="G233" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
-      <c r="D234" s="1"/>
-      <c r="E234" s="1"/>
-      <c r="F234" s="1"/>
-      <c r="G234" s="1"/>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B235" s="1"/>
-      <c r="C235" s="1"/>
-      <c r="D235" s="1"/>
-      <c r="E235" s="1"/>
-      <c r="F235" s="1"/>
-      <c r="G235" s="1"/>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B236" s="1"/>
-      <c r="C236" s="1"/>
-      <c r="D236" s="1"/>
-      <c r="E236" s="1"/>
-      <c r="F236" s="1"/>
-      <c r="G236" s="1"/>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B237" s="1"/>
-      <c r="C237" s="1"/>
-      <c r="D237" s="1"/>
-      <c r="E237" s="1"/>
-      <c r="F237" s="1"/>
-      <c r="G237" s="1"/>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B238" s="1"/>
-      <c r="C238" s="1"/>
-      <c r="D238" s="1"/>
-      <c r="E238" s="1"/>
-      <c r="F238" s="1"/>
-      <c r="G238" s="1"/>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B239" s="1"/>
-      <c r="C239" s="1"/>
-      <c r="D239" s="1"/>
-      <c r="E239" s="1"/>
-      <c r="F239" s="1"/>
-      <c r="G239" s="1"/>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B240" s="1"/>
-      <c r="C240" s="1"/>
-      <c r="D240" s="1"/>
-      <c r="E240" s="1"/>
-      <c r="F240" s="1"/>
-      <c r="G240" s="1"/>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B241" s="1"/>
-      <c r="C241" s="1"/>
-      <c r="D241" s="1"/>
-      <c r="E241" s="1"/>
-      <c r="F241" s="1"/>
-      <c r="G241" s="1"/>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -5973,30 +5855,22 @@
       <c r="D242" s="1">
         <v>8.9931972789115644</v>
       </c>
-      <c r="E242" s="1"/>
-      <c r="F242" s="1"/>
       <c r="G242" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B243" s="1"/>
-      <c r="C243" s="1"/>
-      <c r="D243" s="1"/>
-      <c r="E243" s="1"/>
-      <c r="F243" s="1"/>
       <c r="G243" s="1">
         <v>1828.8</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B244" s="1"/>
       <c r="C244" s="1">
         <v>18</v>
       </c>
@@ -6013,247 +5887,180 @@
         <v>355.6</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B245" s="1">
         <v>289</v>
       </c>
-      <c r="C245" s="1"/>
-      <c r="D245" s="1"/>
-      <c r="E245" s="1"/>
-      <c r="F245" s="1"/>
       <c r="G245" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
       <c r="B246" s="1">
         <v>289</v>
       </c>
-      <c r="C246" s="1"/>
-      <c r="D246" s="1"/>
-      <c r="E246" s="1"/>
-      <c r="F246" s="1"/>
       <c r="G246" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
       <c r="B247" s="1">
         <v>145</v>
       </c>
-      <c r="C247" s="1"/>
-      <c r="D247" s="1"/>
-      <c r="E247" s="1"/>
-      <c r="F247" s="1"/>
       <c r="G247" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
       <c r="B248" s="1">
         <v>145</v>
       </c>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1"/>
-      <c r="F248" s="1"/>
       <c r="G248" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
       <c r="B249" s="1">
         <v>145</v>
       </c>
-      <c r="C249" s="1"/>
-      <c r="D249" s="1"/>
-      <c r="E249" s="1"/>
-      <c r="F249" s="1"/>
       <c r="G249" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B250" s="1">
         <v>289</v>
       </c>
-      <c r="C250" s="1"/>
-      <c r="D250" s="1"/>
-      <c r="E250" s="1"/>
-      <c r="F250" s="1"/>
       <c r="G250" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
       <c r="B251" s="1">
         <v>145</v>
       </c>
-      <c r="C251" s="1"/>
-      <c r="D251" s="1"/>
-      <c r="E251" s="1"/>
-      <c r="F251" s="1"/>
       <c r="G251" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B252" s="1">
         <v>145</v>
       </c>
-      <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
-      <c r="E252" s="1"/>
-      <c r="F252" s="1"/>
       <c r="G252" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B253" s="1">
         <v>289</v>
       </c>
-      <c r="C253" s="1"/>
-      <c r="D253" s="1"/>
-      <c r="E253" s="1"/>
-      <c r="F253" s="1"/>
       <c r="G253" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B254" s="1">
         <v>145</v>
       </c>
-      <c r="C254" s="1"/>
-      <c r="D254" s="1"/>
-      <c r="E254" s="1"/>
-      <c r="F254" s="1"/>
       <c r="G254" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
       <c r="B255" s="1">
         <v>289</v>
       </c>
-      <c r="C255" s="1"/>
-      <c r="D255" s="1"/>
-      <c r="E255" s="1"/>
-      <c r="F255" s="1"/>
       <c r="G255" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
       <c r="B256" s="1">
         <v>289</v>
       </c>
-      <c r="C256" s="1"/>
-      <c r="D256" s="1"/>
-      <c r="E256" s="1"/>
-      <c r="F256" s="1"/>
       <c r="G256" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
       <c r="B257" s="1">
         <v>289</v>
       </c>
-      <c r="C257" s="1"/>
-      <c r="D257" s="1"/>
-      <c r="E257" s="1"/>
-      <c r="F257" s="1"/>
       <c r="G257" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>256</v>
       </c>
       <c r="B258" s="1">
         <v>145</v>
       </c>
-      <c r="C258" s="1"/>
-      <c r="D258" s="1"/>
-      <c r="E258" s="1"/>
-      <c r="F258" s="1"/>
       <c r="G258" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
       <c r="B259" s="1">
         <v>289</v>
       </c>
-      <c r="C259" s="1"/>
-      <c r="D259" s="1"/>
-      <c r="E259" s="1"/>
-      <c r="F259" s="1"/>
       <c r="G259" s="1">
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
-      <c r="E260" s="1"/>
-      <c r="F260" s="1"/>
-      <c r="G260" s="1"/>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B261" s="1"/>
       <c r="C261" s="1">
         <v>10</v>
       </c>
@@ -6270,76 +6077,44 @@
         <v>177.8</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="1"/>
-      <c r="E262" s="1"/>
-      <c r="F262" s="1"/>
-      <c r="G262" s="1"/>
-    </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B263" s="1">
         <v>145</v>
       </c>
-      <c r="C263" s="1"/>
-      <c r="D263" s="1"/>
-      <c r="E263" s="1"/>
-      <c r="F263" s="1"/>
       <c r="G263" s="1">
         <v>3683</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
-      <c r="D264" s="1"/>
-      <c r="E264" s="1"/>
-      <c r="F264" s="1"/>
-      <c r="G264" s="1"/>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B265" s="1"/>
-      <c r="C265" s="1"/>
-      <c r="D265" s="1"/>
-      <c r="E265" s="1"/>
-      <c r="F265" s="1"/>
-      <c r="G265" s="1"/>
-    </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
-      <c r="D266" s="1"/>
-      <c r="E266" s="1"/>
-      <c r="F266" s="1"/>
-      <c r="G266" s="1"/>
-    </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>264</v>
       </c>
       <c r="B267" s="1">
         <v>145</v>
       </c>
-      <c r="C267" s="1"/>
-      <c r="D267" s="1"/>
-      <c r="E267" s="1"/>
-      <c r="F267" s="1"/>
       <c r="G267" s="1">
         <v>3683</v>
       </c>

</xml_diff>

<commit_message>
Finished changes Aug 07
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F877A7FE-A97B-4DF9-9CAD-F14028A33E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6299D852-1DEE-4768-9CF4-D27DD4F8AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="310">
   <si>
     <t>SKU</t>
   </si>
@@ -968,7 +968,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1001,6 +1001,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1081,7 +1088,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1095,6 +1102,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1614,11 +1622,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4826BC9-1387-4C38-A76C-7A9E8593B627}">
   <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B126" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D143" sqref="D143"/>
+      <selection pane="bottomRight" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,15 +1642,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1680,8 +1688,8 @@
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="2">
-        <v>5.2607709750566887</v>
+      <c r="D3" s="7">
+        <v>5.5328798185941039</v>
       </c>
       <c r="E3" s="1">
         <v>101.6</v>
@@ -1931,7 +1939,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="2">
-        <v>9.1609977324263028</v>
+        <v>9.3424036281179141</v>
       </c>
       <c r="E14" s="1">
         <v>76.199999999999989</v>
@@ -1954,7 +1962,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2">
-        <v>18.321995464852609</v>
+        <v>18.684807256235828</v>
       </c>
       <c r="E15" s="1">
         <v>76.199999999999989</v>
@@ -1977,7 +1985,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="2">
-        <v>4.5804988662131514</v>
+        <v>4.6712018140589571</v>
       </c>
       <c r="E16" s="1">
         <v>76.199999999999989</v>
@@ -2337,7 +2345,7 @@
         <v>20</v>
       </c>
       <c r="D31" s="2">
-        <v>7.9552800000000001</v>
+        <v>7.96</v>
       </c>
       <c r="E31" s="1">
         <v>88.899999999999991</v>
@@ -2360,7 +2368,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="2">
-        <v>9.7789999999999988E-2</v>
+        <v>1.0884353741496597</v>
       </c>
       <c r="E32" s="1">
         <v>44.449999999999996</v>
@@ -2386,7 +2394,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="2">
-        <v>14.179549999999999</v>
+        <v>148.02721088435374</v>
       </c>
       <c r="E33" s="1">
         <v>44.45</v>
@@ -2409,7 +2417,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="2">
-        <v>0.29336999999999996</v>
+        <v>3.0839002267573696</v>
       </c>
       <c r="E34" s="1">
         <v>44.449999999999996</v>
@@ -2432,7 +2440,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="2">
-        <v>7.0897749999999995</v>
+        <v>74.013605442176868</v>
       </c>
       <c r="E35" s="1">
         <v>44.45</v>
@@ -3140,7 +3148,7 @@
         <v>20</v>
       </c>
       <c r="D65" s="2">
-        <v>1.7000000000000002</v>
+        <v>0.81632653061224492</v>
       </c>
       <c r="E65" s="1">
         <v>203.2</v>
@@ -3163,7 +3171,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="2">
-        <v>3.4000000000000004</v>
+        <v>2.1768707482993195</v>
       </c>
       <c r="E66" s="1">
         <v>254</v>
@@ -3186,7 +3194,7 @@
         <v>20</v>
       </c>
       <c r="D67" s="2">
-        <v>5.2</v>
+        <v>3.9002267573696141</v>
       </c>
       <c r="E67" s="1">
         <v>215.9</v>
@@ -3209,7 +3217,7 @@
         <v>20</v>
       </c>
       <c r="D68" s="2">
-        <v>6.8000000000000007</v>
+        <v>5.6235827664399096</v>
       </c>
       <c r="E68" s="1">
         <v>203.2</v>
@@ -3301,7 +3309,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="2">
-        <v>1.7999999999999998</v>
+        <v>1.2698412698412698</v>
       </c>
       <c r="E72" s="1">
         <v>254</v>
@@ -3324,7 +3332,7 @@
         <v>20</v>
       </c>
       <c r="D73" s="2">
-        <v>3.5999999999999996</v>
+        <v>2.5396825396825395</v>
       </c>
       <c r="E73" s="1">
         <v>254</v>
@@ -3347,7 +3355,7 @@
         <v>20</v>
       </c>
       <c r="D74" s="2">
-        <v>5.4</v>
+        <v>4.353741496598639</v>
       </c>
       <c r="E74" s="1">
         <v>254</v>
@@ -3370,7 +3378,7 @@
         <v>20</v>
       </c>
       <c r="D75" s="2">
-        <v>7</v>
+        <v>6.0770975056689345</v>
       </c>
       <c r="E75" s="1">
         <v>254</v>
@@ -3566,7 +3574,7 @@
         <v>10</v>
       </c>
       <c r="D83" s="2">
-        <v>8.6182200000000009</v>
+        <v>8.3446712018140587</v>
       </c>
       <c r="E83" s="1">
         <v>76.199999999999989</v>
@@ -3589,7 +3597,7 @@
         <v>10</v>
       </c>
       <c r="D84" s="2">
-        <v>4.2793920000000005</v>
+        <v>4.1723356009070294</v>
       </c>
       <c r="E84" s="1">
         <v>76.199999999999989</v>
@@ -4786,7 +4794,7 @@
         <v>8</v>
       </c>
       <c r="D135" s="2">
-        <v>12.799999999999999</v>
+        <v>10.884353741496598</v>
       </c>
       <c r="E135" s="1">
         <v>88.899999999999991</v>
@@ -4809,7 +4817,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="2">
-        <v>6.4</v>
+        <v>5.4421768707482991</v>
       </c>
       <c r="E136" s="1">
         <v>88.899999999999991</v>
@@ -6362,7 +6370,7 @@
         <v>1</v>
       </c>
       <c r="D206" s="2">
-        <v>6.3492063492063483E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E206" s="1">
         <v>1.016</v>
@@ -6385,7 +6393,7 @@
         <v>1</v>
       </c>
       <c r="D207" s="2">
-        <v>0.63492063492063489</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E207" s="1">
         <v>101.6</v>
@@ -6408,7 +6416,7 @@
         <v>1</v>
       </c>
       <c r="D208" s="2">
-        <v>9.0702947845804989</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E208" s="1">
         <v>152.4</v>
@@ -6427,8 +6435,23 @@
       <c r="A209" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="C209" s="1">
+        <v>1</v>
+      </c>
       <c r="D209" s="2">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E209" s="1">
+        <v>200</v>
+      </c>
+      <c r="F209" s="1">
+        <v>200</v>
+      </c>
+      <c r="G209" s="1">
+        <v>200</v>
+      </c>
+      <c r="H209" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -7155,7 +7178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AEAD2F-541F-42FD-99DA-ABFD75E25C1F}">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished changes Aug 11
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB894878-B774-4798-98F4-823E87D0F0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5ACF9F-983A-4826-8376-BE78AAA2CEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1626,7 +1626,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C210" sqref="C210"/>
+      <selection pane="bottomRight" activeCell="H200" sqref="H200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6393,7 +6393,7 @@
         <v>100</v>
       </c>
       <c r="D207" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="E207" s="1">
         <v>101.6</v>
@@ -6416,7 +6416,7 @@
         <v>1500</v>
       </c>
       <c r="D208" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>7.5</v>
       </c>
       <c r="E208" s="1">
         <v>152.4</v>
@@ -6439,7 +6439,7 @@
         <v>1750</v>
       </c>
       <c r="D209" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>8.75</v>
       </c>
       <c r="E209" s="1">
         <v>200</v>

</xml_diff>

<commit_message>
Fixed bottom row stacking 145s with 289s, works as intended
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\Optimizer\SO Bundles Optimized 251008\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DBD4BC-CA99-407A-AFE0-5A7E4B1B7F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E870A76D-90A6-4670-B7E6-FE09FD1ABF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="4" r:id="rId1"/>
@@ -27,12 +27,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="312">
   <si>
     <t>SKU</t>
   </si>
@@ -1321,9 +1324,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1361,9 +1364,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1396,9 +1399,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,9 +1451,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1610,26 +1647,26 @@
   <dimension ref="A1:I266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B216" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I246" sqref="I246"/>
+      <selection pane="bottomRight" activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.73046875" customWidth="1"/>
-    <col min="9" max="9" width="9.06640625" style="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
       <c r="C1" s="10" t="s">
@@ -1641,7 +1678,7 @@
       <c r="G1" s="11"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1707,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1699,7 +1736,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1725,7 +1762,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +1791,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1777,7 +1814,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,7 +1837,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1837,7 +1874,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1863,7 +1900,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1892,7 +1929,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1918,7 +1955,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1944,7 +1981,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1973,7 +2010,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1999,7 +2036,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2025,7 +2062,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2054,7 +2091,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2080,7 +2117,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2106,7 +2143,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2132,7 +2169,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2161,7 +2198,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2187,7 +2224,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2216,7 +2253,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2242,7 +2279,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2268,7 +2305,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2294,7 +2331,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -2320,7 +2357,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2349,7 +2386,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -2375,7 +2412,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -2401,7 +2438,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -2430,7 +2467,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2453,7 +2490,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2482,7 +2519,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2508,7 +2545,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -2534,7 +2571,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -2560,7 +2597,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -2586,7 +2623,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -2609,7 +2646,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2635,7 +2672,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2661,7 +2698,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2684,7 +2721,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2713,7 +2750,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -2739,7 +2776,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -2762,7 +2799,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -2785,7 +2822,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -2814,7 +2851,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2840,7 +2877,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -2866,7 +2903,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2892,7 +2929,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -2915,7 +2952,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
@@ -2938,7 +2975,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>56</v>
       </c>
@@ -2967,7 +3004,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -2993,7 +3030,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -3022,7 +3059,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -3048,7 +3085,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -3074,7 +3111,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
@@ -3082,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
@@ -3111,7 +3148,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
@@ -3137,7 +3174,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
@@ -3160,7 +3197,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -3183,7 +3220,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
@@ -3206,7 +3243,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -3229,7 +3266,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3289,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
@@ -3275,7 +3312,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>70</v>
       </c>
@@ -3298,7 +3335,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>71</v>
       </c>
@@ -3321,7 +3358,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -3344,7 +3381,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>73</v>
       </c>
@@ -3367,7 +3404,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
@@ -3390,7 +3427,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>75</v>
       </c>
@@ -3413,7 +3450,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -3436,7 +3473,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>77</v>
       </c>
@@ -3459,7 +3496,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>78</v>
       </c>
@@ -3482,7 +3519,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -3505,7 +3542,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -3534,7 +3571,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -3560,7 +3597,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -3589,7 +3626,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -3615,7 +3652,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -3644,7 +3681,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -3670,7 +3707,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -3696,7 +3733,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -3725,7 +3762,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -3751,7 +3788,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -3780,7 +3817,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -3806,7 +3843,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>91</v>
       </c>
@@ -3832,7 +3869,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -3855,7 +3892,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>93</v>
       </c>
@@ -3884,7 +3921,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>94</v>
       </c>
@@ -3910,7 +3947,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>95</v>
       </c>
@@ -3939,7 +3976,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>96</v>
       </c>
@@ -3965,7 +4002,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>97</v>
       </c>
@@ -3991,7 +4028,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>98</v>
       </c>
@@ -4017,7 +4054,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>99</v>
       </c>
@@ -4040,7 +4077,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>100</v>
       </c>
@@ -4048,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>101</v>
       </c>
@@ -4071,7 +4108,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -4097,7 +4134,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>103</v>
       </c>
@@ -4123,7 +4160,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
@@ -4146,7 +4183,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
@@ -4172,7 +4209,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>106</v>
       </c>
@@ -4198,7 +4235,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
@@ -4206,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>108</v>
       </c>
@@ -4214,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>109</v>
       </c>
@@ -4240,7 +4277,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>110</v>
       </c>
@@ -4266,7 +4303,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>111</v>
       </c>
@@ -4292,7 +4329,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>112</v>
       </c>
@@ -4315,7 +4352,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>113</v>
       </c>
@@ -4341,7 +4378,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>114</v>
       </c>
@@ -4367,7 +4404,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>115</v>
       </c>
@@ -4390,7 +4427,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>116</v>
       </c>
@@ -4416,7 +4453,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>117</v>
       </c>
@@ -4442,7 +4479,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>118</v>
       </c>
@@ -4468,7 +4505,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>119</v>
       </c>
@@ -4491,7 +4528,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>120</v>
       </c>
@@ -4517,7 +4554,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>121</v>
       </c>
@@ -4543,7 +4580,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
@@ -4566,7 +4603,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>123</v>
       </c>
@@ -4592,7 +4629,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>124</v>
       </c>
@@ -4618,7 +4655,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>125</v>
       </c>
@@ -4641,7 +4678,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>126</v>
       </c>
@@ -4667,7 +4704,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
@@ -4693,7 +4730,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
@@ -4716,7 +4753,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>129</v>
       </c>
@@ -4742,7 +4779,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>130</v>
       </c>
@@ -4768,7 +4805,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>131</v>
       </c>
@@ -4794,7 +4831,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>132</v>
       </c>
@@ -4802,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>133</v>
       </c>
@@ -4825,7 +4862,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>134</v>
       </c>
@@ -4848,7 +4885,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -4877,7 +4914,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>136</v>
       </c>
@@ -4903,7 +4940,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>137</v>
       </c>
@@ -4926,7 +4963,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>138</v>
       </c>
@@ -4949,7 +4986,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>139</v>
       </c>
@@ -4978,7 +5015,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>140</v>
       </c>
@@ -5004,7 +5041,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>141</v>
       </c>
@@ -5030,7 +5067,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>142</v>
       </c>
@@ -5056,7 +5093,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>143</v>
       </c>
@@ -5079,7 +5116,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>144</v>
       </c>
@@ -5102,7 +5139,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>145</v>
       </c>
@@ -5125,7 +5162,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>146</v>
       </c>
@@ -5151,7 +5188,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
@@ -5177,7 +5214,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>148</v>
       </c>
@@ -5200,7 +5237,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>149</v>
       </c>
@@ -5226,7 +5263,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
@@ -5252,7 +5289,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>151</v>
       </c>
@@ -5275,7 +5312,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>152</v>
       </c>
@@ -5301,7 +5338,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>153</v>
       </c>
@@ -5327,7 +5364,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>154</v>
       </c>
@@ -5350,7 +5387,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>155</v>
       </c>
@@ -5358,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>156</v>
       </c>
@@ -5384,7 +5421,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>157</v>
       </c>
@@ -5410,7 +5447,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>158</v>
       </c>
@@ -5436,7 +5473,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>159</v>
       </c>
@@ -5462,7 +5499,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>160</v>
       </c>
@@ -5485,7 +5522,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>161</v>
       </c>
@@ -5511,7 +5548,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>162</v>
       </c>
@@ -5534,7 +5571,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>163</v>
       </c>
@@ -5557,7 +5594,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>164</v>
       </c>
@@ -5583,7 +5620,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>165</v>
       </c>
@@ -5609,7 +5646,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>166</v>
       </c>
@@ -5632,7 +5669,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>167</v>
       </c>
@@ -5658,7 +5695,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>168</v>
       </c>
@@ -5684,7 +5721,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>169</v>
       </c>
@@ -5710,7 +5747,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>170</v>
       </c>
@@ -5736,7 +5773,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>171</v>
       </c>
@@ -5759,7 +5796,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>172</v>
       </c>
@@ -5785,7 +5822,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>173</v>
       </c>
@@ -5811,7 +5848,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
@@ -5834,7 +5871,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>175</v>
       </c>
@@ -5860,7 +5897,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>176</v>
       </c>
@@ -5886,7 +5923,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>177</v>
       </c>
@@ -5909,7 +5946,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>178</v>
       </c>
@@ -5935,7 +5972,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>179</v>
       </c>
@@ -5958,7 +5995,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>180</v>
       </c>
@@ -5984,7 +6021,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>181</v>
       </c>
@@ -6007,7 +6044,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>182</v>
       </c>
@@ -6033,7 +6070,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>183</v>
       </c>
@@ -6056,7 +6093,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
@@ -6082,7 +6119,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
@@ -6108,7 +6145,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>186</v>
       </c>
@@ -6134,7 +6171,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>187</v>
       </c>
@@ -6157,7 +6194,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>188</v>
       </c>
@@ -6180,7 +6217,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>189</v>
       </c>
@@ -6206,7 +6243,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>190</v>
       </c>
@@ -6229,7 +6266,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>191</v>
       </c>
@@ -6255,7 +6292,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>192</v>
       </c>
@@ -6281,7 +6318,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>193</v>
       </c>
@@ -6307,7 +6344,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>194</v>
       </c>
@@ -6333,7 +6370,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>195</v>
       </c>
@@ -6359,7 +6396,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>196</v>
       </c>
@@ -6382,7 +6419,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
@@ -6408,7 +6445,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>198</v>
       </c>
@@ -6431,7 +6468,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>199</v>
       </c>
@@ -6454,7 +6491,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>200</v>
       </c>
@@ -6462,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>201</v>
       </c>
@@ -6470,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>202</v>
       </c>
@@ -6478,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>203</v>
       </c>
@@ -6486,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>204</v>
       </c>
@@ -6494,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>205</v>
       </c>
@@ -6502,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>206</v>
       </c>
@@ -6510,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>207</v>
       </c>
@@ -6518,7 +6555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>208</v>
       </c>
@@ -6526,7 +6563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>209</v>
       </c>
@@ -6534,122 +6571,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C206" s="1">
-        <v>1</v>
-      </c>
       <c r="D206" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E206" s="1">
-        <v>1.016</v>
-      </c>
-      <c r="F206" s="1">
-        <v>0.254</v>
-      </c>
-      <c r="G206" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="H206" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C207" s="1">
-        <v>100</v>
-      </c>
       <c r="D207" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E207" s="1">
-        <v>101.6</v>
-      </c>
-      <c r="F207" s="1">
-        <v>25.4</v>
-      </c>
-      <c r="G207" s="1">
-        <v>101.6</v>
-      </c>
-      <c r="H207" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C208" s="1">
-        <v>1500</v>
-      </c>
       <c r="D208" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="E208" s="1">
-        <v>152.4</v>
-      </c>
-      <c r="F208" s="1">
-        <v>165.1</v>
-      </c>
-      <c r="G208" s="1">
-        <v>152.4</v>
-      </c>
-      <c r="H208" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C209" s="1">
-        <v>1750</v>
-      </c>
       <c r="D209" s="2">
-        <v>8.75</v>
-      </c>
-      <c r="E209" s="1">
-        <v>200</v>
-      </c>
-      <c r="F209" s="1">
-        <v>200</v>
-      </c>
-      <c r="G209" s="1">
-        <v>200</v>
-      </c>
-      <c r="H209" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C210" s="1">
-        <v>1</v>
-      </c>
       <c r="D210" s="2">
-        <v>1.3605442176870748E-2</v>
-      </c>
-      <c r="E210" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="F210" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="G210" s="1">
-        <v>75</v>
-      </c>
-      <c r="H210" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>213</v>
       </c>
@@ -6675,7 +6637,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>214</v>
       </c>
@@ -6698,7 +6660,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>215</v>
       </c>
@@ -6706,7 +6668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>216</v>
       </c>
@@ -6714,7 +6676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>217</v>
       </c>
@@ -6722,7 +6684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>265</v>
       </c>
@@ -6745,7 +6707,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>218</v>
       </c>
@@ -6753,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>264</v>
       </c>
@@ -6776,7 +6738,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>219</v>
       </c>
@@ -6784,7 +6746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>220</v>
       </c>
@@ -6792,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>221</v>
       </c>
@@ -6800,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>222</v>
       </c>
@@ -6808,7 +6770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>223</v>
       </c>
@@ -6816,7 +6778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>224</v>
       </c>
@@ -6845,7 +6807,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>225</v>
       </c>
@@ -6874,7 +6836,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>226</v>
       </c>
@@ -6900,7 +6862,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>227</v>
       </c>
@@ -6929,7 +6891,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>228</v>
       </c>
@@ -6958,7 +6920,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>229</v>
       </c>
@@ -6984,7 +6946,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>230</v>
       </c>
@@ -7010,7 +6972,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>231</v>
       </c>
@@ -7021,7 +6983,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>232</v>
       </c>
@@ -7032,7 +6994,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>233</v>
       </c>
@@ -7040,7 +7002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>1</v>
       </c>
@@ -7048,7 +7010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
@@ -7056,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
@@ -7064,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
@@ -7072,7 +7034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
@@ -7080,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
@@ -7088,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>2</v>
       </c>
@@ -7096,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
@@ -7104,7 +7066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -7124,7 +7086,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
@@ -7147,7 +7109,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
@@ -7170,7 +7132,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
@@ -7178,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
@@ -7186,7 +7148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
@@ -7194,7 +7156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
@@ -7202,7 +7164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
@@ -7210,7 +7172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
@@ -7218,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
@@ -7226,7 +7188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
@@ -7234,7 +7196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
@@ -7242,7 +7204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
@@ -7250,7 +7212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
@@ -7258,7 +7220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
@@ -7266,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
@@ -7274,7 +7236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>256</v>
       </c>
@@ -7282,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
@@ -7290,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
@@ -7298,30 +7260,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C261" s="1">
-        <v>10</v>
-      </c>
       <c r="D261" s="2">
-        <v>0.90702947845804993</v>
-      </c>
-      <c r="E261" s="1">
-        <v>127</v>
-      </c>
-      <c r="F261" s="1">
-        <v>25.4</v>
-      </c>
-      <c r="G261" s="1">
-        <v>177.8</v>
-      </c>
-      <c r="H261" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>259</v>
       </c>
@@ -7329,7 +7276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>260</v>
       </c>
@@ -7337,7 +7284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>261</v>
       </c>
@@ -7345,7 +7292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>262</v>
       </c>
@@ -7353,7 +7300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>263</v>
       </c>
@@ -7381,184 +7328,184 @@
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>307</v>
       </c>

</xml_diff>

<commit_message>
Finished changes Dec 12
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\Optimizer\Optimizer SW 251027\_internal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\Optimizer\Optimizer SW 251202\_internal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26CAA866-DE83-4A68-A6A0-6183E87C30B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5BDE06-14A4-4A41-8D1A-B85A2613EF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="10650" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="1" r:id="rId1"/>
     <sheet name="MACH1_SKUs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="327">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -996,13 +1009,19 @@
   </si>
   <si>
     <t>WGY</t>
+  </si>
+  <si>
+    <t>6V.157</t>
+  </si>
+  <si>
+    <t>TP4ALP.12X96</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1016,13 +1035,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1052,11 +1089,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1359,11 +1398,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I271"/>
+  <dimension ref="A1:I273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="L247" sqref="L247"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -1508,49 +1559,57 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
         <v>1.387755102040816E-2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>25.4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>14.2875</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>76.199999999999989</v>
       </c>
-      <c r="H6" t="s">
-        <v>19</v>
+      <c r="H6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
         <v>2.3492063492063491E-2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>25.4</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>14.2875</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>127</v>
       </c>
-      <c r="H7" t="s">
-        <v>19</v>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -2205,6 +2264,9 @@
       <c r="H32" t="s">
         <v>19</v>
       </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
@@ -2514,6 +2576,9 @@
       <c r="H44" t="s">
         <v>19</v>
       </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
@@ -2537,6 +2602,9 @@
       <c r="H45" t="s">
         <v>19</v>
       </c>
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
@@ -2912,6 +2980,9 @@
       <c r="H60" t="s">
         <v>19</v>
       </c>
+      <c r="I60" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
@@ -2935,6 +3006,9 @@
       <c r="H61" t="s">
         <v>19</v>
       </c>
+      <c r="I61" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
@@ -2958,6 +3032,9 @@
       <c r="H62" t="s">
         <v>19</v>
       </c>
+      <c r="I62" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
@@ -2981,6 +3058,9 @@
       <c r="H63" t="s">
         <v>19</v>
       </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
@@ -3004,6 +3084,9 @@
       <c r="H64" t="s">
         <v>19</v>
       </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
@@ -3027,6 +3110,9 @@
       <c r="H65" t="s">
         <v>19</v>
       </c>
+      <c r="I65" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
@@ -3050,6 +3136,9 @@
       <c r="H66" t="s">
         <v>19</v>
       </c>
+      <c r="I66" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
@@ -3073,6 +3162,9 @@
       <c r="H67" t="s">
         <v>19</v>
       </c>
+      <c r="I67" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
@@ -3096,6 +3188,9 @@
       <c r="H68" t="s">
         <v>19</v>
       </c>
+      <c r="I68" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
@@ -3119,6 +3214,9 @@
       <c r="H69" t="s">
         <v>19</v>
       </c>
+      <c r="I69" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
@@ -3142,6 +3240,9 @@
       <c r="H70" t="s">
         <v>19</v>
       </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
@@ -3165,6 +3266,9 @@
       <c r="H71" t="s">
         <v>19</v>
       </c>
+      <c r="I71" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
@@ -3188,6 +3292,9 @@
       <c r="H72" t="s">
         <v>19</v>
       </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
@@ -3211,6 +3318,9 @@
       <c r="H73" t="s">
         <v>19</v>
       </c>
+      <c r="I73" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
@@ -3234,6 +3344,9 @@
       <c r="H74" t="s">
         <v>19</v>
       </c>
+      <c r="I74" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
@@ -3257,6 +3370,9 @@
       <c r="H75" t="s">
         <v>19</v>
       </c>
+      <c r="I75" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
@@ -3607,6 +3723,9 @@
       <c r="H88" t="s">
         <v>19</v>
       </c>
+      <c r="I88" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
@@ -3794,14 +3913,23 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
+      <c r="A96" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D96">
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -3823,8 +3951,11 @@
       <c r="H97" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -3850,7 +3981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -3876,7 +4007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -3899,7 +4030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>118</v>
       </c>
@@ -3925,7 +4056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>119</v>
       </c>
@@ -3951,7 +4082,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>120</v>
       </c>
@@ -3959,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -3967,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>122</v>
       </c>
@@ -3993,7 +4124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>123</v>
       </c>
@@ -4019,7 +4150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>124</v>
       </c>
@@ -4045,7 +4176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>125</v>
       </c>
@@ -4068,7 +4199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>126</v>
       </c>
@@ -4094,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>127</v>
       </c>
@@ -4120,7 +4251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>128</v>
       </c>
@@ -4143,7 +4274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -4169,7 +4300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>130</v>
       </c>
@@ -4195,7 +4326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -4221,7 +4352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>132</v>
       </c>
@@ -4244,7 +4375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>133</v>
       </c>
@@ -4270,7 +4401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>134</v>
       </c>
@@ -4296,7 +4427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -4319,7 +4450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>136</v>
       </c>
@@ -4345,7 +4476,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>137</v>
       </c>
@@ -4371,7 +4502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -4394,7 +4525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>139</v>
       </c>
@@ -4420,7 +4551,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>140</v>
       </c>
@@ -4446,7 +4577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -4469,7 +4600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -4495,7 +4626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -4521,7 +4652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>144</v>
       </c>
@@ -4547,27 +4678,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A128" t="s">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A128" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C128">
+      <c r="B128" s="3"/>
+      <c r="C128" s="3">
         <v>100</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="3">
         <v>2.2321428571428572</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="3">
         <v>203.2</v>
       </c>
-      <c r="F128">
+      <c r="F128" s="3">
         <v>101.6</v>
       </c>
-      <c r="G128">
+      <c r="G128" s="3">
         <v>228.6</v>
       </c>
-      <c r="H128" t="s">
-        <v>19</v>
+      <c r="H128" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
@@ -4869,6 +5004,9 @@
       <c r="H140" t="s">
         <v>19</v>
       </c>
+      <c r="I140" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
@@ -4892,6 +5030,9 @@
       <c r="H141" t="s">
         <v>19</v>
       </c>
+      <c r="I141" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
@@ -4968,7 +5109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>162</v>
       </c>
@@ -4994,7 +5135,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -5020,7 +5161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -5043,7 +5184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>165</v>
       </c>
@@ -5069,7 +5210,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>166</v>
       </c>
@@ -5095,7 +5236,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>167</v>
       </c>
@@ -5118,7 +5259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>168</v>
       </c>
@@ -5126,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>169</v>
       </c>
@@ -5152,7 +5293,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>170</v>
       </c>
@@ -5178,7 +5319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>171</v>
       </c>
@@ -5204,7 +5345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>172</v>
       </c>
@@ -5230,7 +5371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>173</v>
       </c>
@@ -5253,7 +5394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>174</v>
       </c>
@@ -5279,7 +5420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>175</v>
       </c>
@@ -5302,7 +5443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>176</v>
       </c>
@@ -5324,8 +5465,11 @@
       <c r="H159" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I159" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>177</v>
       </c>
@@ -5534,11 +5678,11 @@
       <c r="B168">
         <v>145</v>
       </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-      <c r="D168">
-        <v>4.0144700000000002</v>
+      <c r="C168" s="2">
+        <v>4</v>
+      </c>
+      <c r="D168" s="2">
+        <v>16.056999999999999</v>
       </c>
       <c r="E168">
         <v>168.27500000000001</v>
@@ -5560,11 +5704,11 @@
       <c r="B169">
         <v>289</v>
       </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-      <c r="D169">
-        <v>8.00169</v>
+      <c r="C169" s="2">
+        <v>4</v>
+      </c>
+      <c r="D169" s="2">
+        <v>32.006999999999998</v>
       </c>
       <c r="E169">
         <v>168.27500000000001</v>
@@ -5583,11 +5727,11 @@
       <c r="A170" t="s">
         <v>187</v>
       </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-      <c r="D170">
-        <v>2.0072350000000001</v>
+      <c r="C170" s="2">
+        <v>4</v>
+      </c>
+      <c r="D170" s="2">
+        <v>8.0280000000000005</v>
       </c>
       <c r="E170">
         <v>168.27500000000001</v>
@@ -5629,25 +5773,25 @@
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A172" t="s">
+      <c r="A172" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="3">
         <v>145</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="3">
         <v>8</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="3">
         <v>23.945578231292519</v>
       </c>
-      <c r="E172">
+      <c r="E172" s="3">
         <v>177.8</v>
       </c>
-      <c r="F172">
-        <v>50.8</v>
-      </c>
-      <c r="G172">
+      <c r="F172" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="G172" s="3">
         <v>3683</v>
       </c>
       <c r="H172" t="s">
@@ -5655,98 +5799,98 @@
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A173" t="s">
+      <c r="A173" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3">
+        <v>8</v>
+      </c>
+      <c r="D173" s="3">
+        <v>25.92728125733052</v>
+      </c>
+      <c r="E173" s="3">
+        <v>177.8</v>
+      </c>
+      <c r="F173" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="G173" s="3">
+        <v>3987.7999999999997</v>
+      </c>
+      <c r="H173" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A174" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C173">
+      <c r="B174" s="3"/>
+      <c r="C174" s="3">
         <v>8</v>
       </c>
-      <c r="D173">
+      <c r="D174" s="3">
         <v>39.936915942847733</v>
       </c>
-      <c r="E173">
+      <c r="E174" s="3">
         <v>177.8</v>
       </c>
-      <c r="F173">
-        <v>50.8</v>
-      </c>
-      <c r="G173">
+      <c r="F174" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="G174" s="3">
         <v>6121.4</v>
       </c>
-      <c r="H173" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
+      <c r="H174" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A175" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B174">
+      <c r="B175" s="3">
         <v>289</v>
       </c>
-      <c r="C174">
+      <c r="C175" s="3">
         <v>8</v>
       </c>
-      <c r="D174">
+      <c r="D175" s="3">
         <v>47.89115646258503</v>
       </c>
-      <c r="E174">
+      <c r="E175" s="3">
         <v>177.8</v>
       </c>
-      <c r="F174">
-        <v>50.8</v>
-      </c>
-      <c r="G174">
+      <c r="F175" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="G175" s="3">
         <v>7340.5999999999995</v>
       </c>
-      <c r="H174" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A175" t="s">
+      <c r="H175" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A176" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C175">
+      <c r="B176" s="3"/>
+      <c r="C176" s="3">
         <v>8</v>
       </c>
-      <c r="D175">
+      <c r="D176" s="3">
         <v>11.972789115646259</v>
       </c>
-      <c r="E175">
+      <c r="E176" s="3">
         <v>177.8</v>
       </c>
-      <c r="F175">
-        <v>50.8</v>
-      </c>
-      <c r="G175">
+      <c r="F176" s="3">
+        <v>50.8</v>
+      </c>
+      <c r="G176" s="3">
         <v>1828.8</v>
-      </c>
-      <c r="H175" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A176" t="s">
-        <v>193</v>
-      </c>
-      <c r="B176">
-        <v>145</v>
-      </c>
-      <c r="C176">
-        <v>8</v>
-      </c>
-      <c r="D176">
-        <v>23.945578231292519</v>
-      </c>
-      <c r="E176">
-        <v>177.8</v>
-      </c>
-      <c r="F176">
-        <v>50.8</v>
-      </c>
-      <c r="G176">
-        <v>3683</v>
       </c>
       <c r="H176" t="s">
         <v>19</v>
@@ -5754,13 +5898,16 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="B177">
+        <v>145</v>
       </c>
       <c r="C177">
         <v>8</v>
       </c>
       <c r="D177">
-        <v>41.925476072782047</v>
+        <v>23.945578231292519</v>
       </c>
       <c r="E177">
         <v>177.8</v>
@@ -5769,7 +5916,7 @@
         <v>50.8</v>
       </c>
       <c r="G177">
-        <v>6426.2</v>
+        <v>3683</v>
       </c>
       <c r="H177" t="s">
         <v>19</v>
@@ -5777,16 +5924,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>195</v>
-      </c>
-      <c r="B178">
-        <v>289</v>
+        <v>194</v>
       </c>
       <c r="C178">
         <v>8</v>
       </c>
       <c r="D178">
-        <v>47.89115646258503</v>
+        <v>41.925476072782047</v>
       </c>
       <c r="E178">
         <v>177.8</v>
@@ -5795,7 +5939,7 @@
         <v>50.8</v>
       </c>
       <c r="G178">
-        <v>7340.5999999999995</v>
+        <v>6426.2</v>
       </c>
       <c r="H178" t="s">
         <v>19</v>
@@ -5803,13 +5947,16 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="B179">
+        <v>289</v>
       </c>
       <c r="C179">
         <v>8</v>
       </c>
       <c r="D179">
-        <v>11.972789115646259</v>
+        <v>47.89115646258503</v>
       </c>
       <c r="E179">
         <v>177.8</v>
@@ -5818,7 +5965,7 @@
         <v>50.8</v>
       </c>
       <c r="G179">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H179" t="s">
         <v>19</v>
@@ -5826,16 +5973,13 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>197</v>
-      </c>
-      <c r="B180">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="C180">
         <v>8</v>
       </c>
       <c r="D180">
-        <v>23.945578231292519</v>
+        <v>11.972789115646259</v>
       </c>
       <c r="E180">
         <v>177.8</v>
@@ -5844,7 +5988,7 @@
         <v>50.8</v>
       </c>
       <c r="G180">
-        <v>3683</v>
+        <v>1828.8</v>
       </c>
       <c r="H180" t="s">
         <v>19</v>
@@ -5852,16 +5996,16 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B181">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C181">
         <v>8</v>
       </c>
       <c r="D181">
-        <v>47.89115646258503</v>
+        <v>23.945578231292519</v>
       </c>
       <c r="E181">
         <v>177.8</v>
@@ -5870,7 +6014,7 @@
         <v>50.8</v>
       </c>
       <c r="G181">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H181" t="s">
         <v>19</v>
@@ -5878,16 +6022,16 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B182">
-        <v>145</v>
+        <v>289</v>
       </c>
       <c r="C182">
         <v>8</v>
       </c>
       <c r="D182">
-        <v>25.396825396825399</v>
+        <v>47.89115646258503</v>
       </c>
       <c r="E182">
         <v>177.8</v>
@@ -5896,7 +6040,7 @@
         <v>50.8</v>
       </c>
       <c r="G182">
-        <v>3683</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H182" t="s">
         <v>19</v>
@@ -5904,13 +6048,16 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="B183">
+        <v>145</v>
       </c>
       <c r="C183">
         <v>8</v>
       </c>
       <c r="D183">
-        <v>33.921019388147407</v>
+        <v>25.396825396825399</v>
       </c>
       <c r="E183">
         <v>177.8</v>
@@ -5919,7 +6066,7 @@
         <v>50.8</v>
       </c>
       <c r="G183">
-        <v>4902.2</v>
+        <v>3683</v>
       </c>
       <c r="H183" t="s">
         <v>19</v>
@@ -5927,13 +6074,13 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C184">
         <v>8</v>
       </c>
       <c r="D184">
-        <v>44.466414016587017</v>
+        <v>33.921019388147407</v>
       </c>
       <c r="E184">
         <v>177.8</v>
@@ -5942,7 +6089,7 @@
         <v>50.8</v>
       </c>
       <c r="G184">
-        <v>6426.2</v>
+        <v>4902.2</v>
       </c>
       <c r="H184" t="s">
         <v>19</v>
@@ -5950,16 +6097,13 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
-        <v>202</v>
-      </c>
-      <c r="B185">
-        <v>289</v>
+        <v>201</v>
       </c>
       <c r="C185">
         <v>8</v>
       </c>
       <c r="D185">
-        <v>50.793650793650791</v>
+        <v>44.466414016587017</v>
       </c>
       <c r="E185">
         <v>177.8</v>
@@ -5968,7 +6112,7 @@
         <v>50.8</v>
       </c>
       <c r="G185">
-        <v>7340.5999999999995</v>
+        <v>6426.2</v>
       </c>
       <c r="H185" t="s">
         <v>19</v>
@@ -5976,13 +6120,16 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="B186">
+        <v>289</v>
       </c>
       <c r="C186">
         <v>8</v>
       </c>
       <c r="D186">
-        <v>12.698412698412699</v>
+        <v>50.793650793650791</v>
       </c>
       <c r="E186">
         <v>177.8</v>
@@ -5991,7 +6138,7 @@
         <v>50.8</v>
       </c>
       <c r="G186">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H186" t="s">
         <v>19</v>
@@ -5999,25 +6146,22 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>204</v>
-      </c>
-      <c r="B187">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="C187">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D187">
-        <v>3.3147000000000002</v>
+        <v>12.698412698412699</v>
       </c>
       <c r="E187">
-        <v>193.67500000000001</v>
+        <v>177.8</v>
       </c>
       <c r="F187">
-        <v>11.112500000000001</v>
+        <v>50.8</v>
       </c>
       <c r="G187">
-        <v>3683</v>
+        <v>1828.8</v>
       </c>
       <c r="H187" t="s">
         <v>19</v>
@@ -6025,22 +6169,22 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B188">
         <v>145</v>
       </c>
-      <c r="C188">
-        <v>1</v>
-      </c>
-      <c r="D188">
-        <v>3.7308789999999998</v>
+      <c r="C188" s="2">
+        <v>8</v>
+      </c>
+      <c r="D188" s="2">
+        <v>26.517600000000002</v>
       </c>
       <c r="E188">
-        <v>177.8</v>
+        <v>193.67500000000001</v>
       </c>
       <c r="F188">
-        <v>4</v>
+        <v>11.112500000000001</v>
       </c>
       <c r="G188">
         <v>3683</v>
@@ -6051,16 +6195,16 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B189">
-        <v>289</v>
-      </c>
-      <c r="C189">
-        <v>1</v>
-      </c>
-      <c r="D189">
-        <v>7.4364330000000001</v>
+        <v>145</v>
+      </c>
+      <c r="C189" s="2">
+        <v>8</v>
+      </c>
+      <c r="D189" s="2">
+        <v>29.847000000000001</v>
       </c>
       <c r="E189">
         <v>177.8</v>
@@ -6069,7 +6213,7 @@
         <v>4</v>
       </c>
       <c r="G189">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H189" t="s">
         <v>19</v>
@@ -6077,25 +6221,25 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B190">
-        <v>145</v>
-      </c>
-      <c r="C190">
+        <v>289</v>
+      </c>
+      <c r="C190" s="2">
         <v>8</v>
       </c>
-      <c r="D190">
-        <v>37.124639999999999</v>
+      <c r="D190" s="2">
+        <v>59.491199999999999</v>
       </c>
       <c r="E190">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="F190">
-        <v>50.8</v>
+        <v>4</v>
       </c>
       <c r="G190">
-        <v>3683</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H190" t="s">
         <v>19</v>
@@ -6103,16 +6247,16 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B191">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C191">
         <v>8</v>
       </c>
       <c r="D191">
-        <v>73.993247999999994</v>
+        <v>37.124639999999999</v>
       </c>
       <c r="E191">
         <v>228.6</v>
@@ -6121,7 +6265,7 @@
         <v>50.8</v>
       </c>
       <c r="G191">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H191" t="s">
         <v>19</v>
@@ -6129,13 +6273,16 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
-        <v>209</v>
+        <v>208</v>
+      </c>
+      <c r="B192">
+        <v>289</v>
       </c>
       <c r="C192">
         <v>8</v>
       </c>
       <c r="D192">
-        <v>18.434304000000001</v>
+        <v>73.993247999999994</v>
       </c>
       <c r="E192">
         <v>228.6</v>
@@ -6144,70 +6291,70 @@
         <v>50.8</v>
       </c>
       <c r="G192">
+        <v>7340.5999999999995</v>
+      </c>
+      <c r="H192" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A193" t="s">
+        <v>209</v>
+      </c>
+      <c r="C193">
+        <v>8</v>
+      </c>
+      <c r="D193">
+        <v>18.434304000000001</v>
+      </c>
+      <c r="E193">
+        <v>228.6</v>
+      </c>
+      <c r="F193">
+        <v>50.8</v>
+      </c>
+      <c r="G193">
         <v>1828.8</v>
       </c>
-      <c r="H192" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A193" t="s">
+      <c r="H193" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A194" t="s">
         <v>210</v>
       </c>
-      <c r="B193">
+      <c r="B194">
         <v>145</v>
       </c>
-      <c r="C193">
+      <c r="C194">
         <v>1</v>
       </c>
-      <c r="D193">
+      <c r="D194">
         <v>4.0107869999999997</v>
       </c>
-      <c r="E193">
+      <c r="E194">
         <v>219.07499999999999</v>
       </c>
-      <c r="F193">
+      <c r="F194">
         <v>11.112500000000001</v>
       </c>
-      <c r="G193">
+      <c r="G194">
         <v>3683</v>
       </c>
-      <c r="H193" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A194" t="s">
+      <c r="H194" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A195" t="s">
         <v>211</v>
-      </c>
-      <c r="C194">
-        <v>53</v>
-      </c>
-      <c r="D194">
-        <v>4.353741496598639</v>
-      </c>
-      <c r="E194">
-        <v>165.1</v>
-      </c>
-      <c r="F194">
-        <v>114.3</v>
-      </c>
-      <c r="G194">
-        <v>127</v>
-      </c>
-      <c r="H194" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A195" t="s">
-        <v>212</v>
       </c>
       <c r="C195">
         <v>53</v>
       </c>
       <c r="D195">
-        <v>5.2244897959183669</v>
+        <v>4.353741496598639</v>
       </c>
       <c r="E195">
         <v>165.1</v>
@@ -6216,44 +6363,50 @@
         <v>114.3</v>
       </c>
       <c r="G195">
+        <v>127</v>
+      </c>
+      <c r="H195" t="s">
+        <v>19</v>
+      </c>
+      <c r="I195" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A196" t="s">
+        <v>212</v>
+      </c>
+      <c r="C196">
+        <v>53</v>
+      </c>
+      <c r="D196">
+        <v>5.2244897959183669</v>
+      </c>
+      <c r="E196">
+        <v>165.1</v>
+      </c>
+      <c r="F196">
+        <v>114.3</v>
+      </c>
+      <c r="G196">
         <v>152.4</v>
       </c>
-      <c r="H195" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A196" t="s">
+      <c r="H196" t="s">
+        <v>19</v>
+      </c>
+      <c r="I196" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A197" t="s">
         <v>213</v>
       </c>
-      <c r="C196">
+      <c r="C197">
         <v>1</v>
       </c>
-      <c r="D196">
+      <c r="D197">
         <v>6.1160714285714277E-2</v>
-      </c>
-      <c r="E196">
-        <v>50.8</v>
-      </c>
-      <c r="F196">
-        <v>19.05</v>
-      </c>
-      <c r="G196">
-        <v>25.4</v>
-      </c>
-      <c r="H196" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A197" t="s">
-        <v>214</v>
-      </c>
-      <c r="C197">
-        <v>20</v>
-      </c>
-      <c r="D197">
-        <v>1.223214285714286</v>
       </c>
       <c r="E197">
         <v>50.8</v>
@@ -6262,44 +6415,44 @@
         <v>19.05</v>
       </c>
       <c r="G197">
+        <v>25.4</v>
+      </c>
+      <c r="H197" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A198" t="s">
+        <v>214</v>
+      </c>
+      <c r="C198">
+        <v>20</v>
+      </c>
+      <c r="D198">
+        <v>1.223214285714286</v>
+      </c>
+      <c r="E198">
+        <v>50.8</v>
+      </c>
+      <c r="F198">
+        <v>19.05</v>
+      </c>
+      <c r="G198">
         <v>100</v>
       </c>
-      <c r="H197" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A198" t="s">
+      <c r="H198" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A199" t="s">
         <v>215</v>
-      </c>
-      <c r="C198">
-        <v>1</v>
-      </c>
-      <c r="D198">
-        <v>0.31473214285714279</v>
-      </c>
-      <c r="E198">
-        <v>38.099999999999987</v>
-      </c>
-      <c r="F198">
-        <v>38.099999999999987</v>
-      </c>
-      <c r="G198">
-        <v>254</v>
-      </c>
-      <c r="H198" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A199" t="s">
-        <v>216</v>
       </c>
       <c r="C199">
         <v>1</v>
       </c>
       <c r="D199">
-        <v>0.37767857142857131</v>
+        <v>0.31473214285714279</v>
       </c>
       <c r="E199">
         <v>38.099999999999987</v>
@@ -6308,21 +6461,21 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G199">
-        <v>304.8</v>
+        <v>254</v>
       </c>
       <c r="H199" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C200">
         <v>1</v>
       </c>
       <c r="D200">
-        <v>6.2946428571428556E-2</v>
+        <v>0.37767857142857131</v>
       </c>
       <c r="E200">
         <v>38.099999999999987</v>
@@ -6331,21 +6484,21 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G200">
-        <v>50.8</v>
+        <v>304.8</v>
       </c>
       <c r="H200" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C201">
         <v>1</v>
       </c>
       <c r="D201">
-        <v>0.12589285714285711</v>
+        <v>6.2946428571428556E-2</v>
       </c>
       <c r="E201">
         <v>38.099999999999987</v>
@@ -6354,21 +6507,24 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G201">
-        <v>101.6</v>
+        <v>50.8</v>
       </c>
       <c r="H201" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I201" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C202">
         <v>1</v>
       </c>
       <c r="D202">
-        <v>0.18883928571428571</v>
+        <v>0.12589285714285711</v>
       </c>
       <c r="E202">
         <v>38.099999999999987</v>
@@ -6377,21 +6533,24 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G202">
-        <v>152.4</v>
+        <v>101.6</v>
       </c>
       <c r="H202" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I202" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C203">
         <v>1</v>
       </c>
       <c r="D203">
-        <v>0.25178571428571422</v>
+        <v>0.18883928571428571</v>
       </c>
       <c r="E203">
         <v>38.099999999999987</v>
@@ -6400,142 +6559,163 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G203">
-        <v>203.2</v>
+        <v>152.4</v>
       </c>
       <c r="H203" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I203" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C204">
         <v>1</v>
       </c>
       <c r="D204">
-        <v>8.0357142857142847</v>
+        <v>0.25178571428571422</v>
       </c>
       <c r="E204">
-        <v>50.8</v>
+        <v>38.099999999999987</v>
       </c>
       <c r="F204">
-        <v>50.8</v>
+        <v>38.099999999999987</v>
       </c>
       <c r="G204">
-        <v>7340.5999999999995</v>
+        <v>203.2</v>
       </c>
       <c r="H204" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I204" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C205">
         <v>1</v>
       </c>
       <c r="D205">
+        <v>8.0357142857142847</v>
+      </c>
+      <c r="E205">
+        <v>50.8</v>
+      </c>
+      <c r="F205">
+        <v>50.8</v>
+      </c>
+      <c r="G205">
+        <v>7340.5999999999995</v>
+      </c>
+      <c r="H205" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>222</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
         <v>2.0019772614928319</v>
       </c>
-      <c r="E205">
-        <v>50.8</v>
-      </c>
-      <c r="F205">
-        <v>50.8</v>
-      </c>
-      <c r="G205">
+      <c r="E206">
+        <v>50.8</v>
+      </c>
+      <c r="F206">
+        <v>50.8</v>
+      </c>
+      <c r="G206">
         <v>1828.8</v>
       </c>
-      <c r="H205" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A206" t="s">
+      <c r="H206" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A207" t="s">
         <v>223</v>
-      </c>
-      <c r="D206">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A207" t="s">
-        <v>224</v>
       </c>
       <c r="D207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I207" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D208">
         <v>0</v>
       </c>
+      <c r="I208" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D209">
         <v>0</v>
       </c>
+      <c r="I209" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D210">
         <v>0</v>
       </c>
+      <c r="I210" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
-        <v>228</v>
-      </c>
-      <c r="B211">
-        <v>289</v>
-      </c>
-      <c r="C211">
-        <v>1</v>
+        <v>227</v>
       </c>
       <c r="D211">
-        <v>10.057169999999999</v>
-      </c>
-      <c r="E211">
-        <v>101.6</v>
-      </c>
-      <c r="F211">
-        <v>41.274999999999999</v>
-      </c>
-      <c r="G211">
-        <v>7340.5999999999995</v>
-      </c>
-      <c r="H211" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="I211" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="B212">
+        <v>289</v>
       </c>
       <c r="C212">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D212">
-        <v>1.45124716553288</v>
+        <v>10.057169999999999</v>
       </c>
       <c r="E212">
-        <v>190.5</v>
+        <v>101.6</v>
       </c>
       <c r="F212">
-        <v>101.6</v>
+        <v>41.274999999999999</v>
       </c>
       <c r="G212">
-        <v>228.6</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H212" t="s">
         <v>19</v>
@@ -6543,22 +6723,22 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C213">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D213">
-        <v>3.258928571428571E-2</v>
+        <v>1.45124716553288</v>
       </c>
       <c r="E213">
-        <v>38.099999999999987</v>
+        <v>190.5</v>
       </c>
       <c r="F213">
-        <v>25.4</v>
+        <v>101.6</v>
       </c>
       <c r="G213">
-        <v>63.5</v>
+        <v>228.6</v>
       </c>
       <c r="H213" t="s">
         <v>19</v>
@@ -6569,22 +6749,22 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C214">
         <v>1</v>
       </c>
       <c r="D214">
-        <v>2.2321428571428572</v>
+        <v>3.258928571428571E-2</v>
       </c>
       <c r="E214">
-        <v>76.199999999999989</v>
+        <v>38.099999999999987</v>
       </c>
       <c r="F214">
-        <v>19.05</v>
+        <v>25.4</v>
       </c>
       <c r="G214">
-        <v>1828.8</v>
+        <v>63.5</v>
       </c>
       <c r="H214" t="s">
         <v>19</v>
@@ -6595,56 +6775,56 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
       </c>
       <c r="D215">
-        <v>0</v>
+        <v>2.2321428571428572</v>
+      </c>
+      <c r="E215">
+        <v>76.199999999999989</v>
+      </c>
+      <c r="F215">
+        <v>19.05</v>
+      </c>
+      <c r="G215">
+        <v>1828.8</v>
+      </c>
+      <c r="H215" t="s">
+        <v>19</v>
+      </c>
+      <c r="I215" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
-        <v>233</v>
-      </c>
-      <c r="C216">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="D216">
-        <v>3.5714285714285712</v>
-      </c>
-      <c r="E216">
-        <v>76.199999999999989</v>
-      </c>
-      <c r="F216">
-        <v>19.05</v>
-      </c>
-      <c r="G216">
-        <v>1828.8</v>
-      </c>
-      <c r="H216" t="s">
-        <v>19</v>
-      </c>
-      <c r="I216" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C217">
         <v>1</v>
       </c>
       <c r="D217">
-        <v>5.3571428571428568</v>
+        <v>3.5714285714285712</v>
       </c>
       <c r="E217">
-        <v>101.6</v>
+        <v>76.199999999999989</v>
       </c>
       <c r="F217">
         <v>19.05</v>
       </c>
       <c r="G217">
-        <v>3657.6</v>
+        <v>1828.8</v>
       </c>
       <c r="H217" t="s">
         <v>19</v>
@@ -6655,71 +6835,71 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C218">
         <v>1</v>
       </c>
       <c r="D218">
-        <v>0</v>
+        <v>5.3571428571428568</v>
       </c>
       <c r="E218">
-        <v>203.2</v>
+        <v>101.6</v>
       </c>
       <c r="F218">
-        <v>88.899999999999991</v>
+        <v>19.05</v>
       </c>
       <c r="G218">
-        <v>508</v>
+        <v>3657.6</v>
       </c>
       <c r="H218" t="s">
         <v>19</v>
+      </c>
+      <c r="I218" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C219">
         <v>1</v>
       </c>
       <c r="D219">
-        <v>6.9196428571428568</v>
+        <v>0</v>
       </c>
       <c r="E219">
-        <v>101.6</v>
+        <v>203.2</v>
       </c>
       <c r="F219">
-        <v>19.05</v>
+        <v>88.899999999999991</v>
       </c>
       <c r="G219">
-        <v>4876.7999999999993</v>
+        <v>508</v>
       </c>
       <c r="H219" t="s">
         <v>19</v>
-      </c>
-      <c r="I219" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C220">
         <v>1</v>
       </c>
       <c r="D220">
-        <v>0.1397321428571428</v>
+        <v>6.9196428571428568</v>
       </c>
       <c r="E220">
-        <v>50.8</v>
+        <v>101.6</v>
       </c>
       <c r="F220">
-        <v>25.4</v>
+        <v>19.05</v>
       </c>
       <c r="G220">
-        <v>101.6</v>
+        <v>4876.7999999999993</v>
       </c>
       <c r="H220" t="s">
         <v>19</v>
@@ -6730,93 +6910,90 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C221">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D221">
-        <v>9.9773242630385486</v>
+        <v>0.1397321428571428</v>
       </c>
       <c r="E221">
-        <v>165.1</v>
+        <v>50.8</v>
       </c>
       <c r="F221">
-        <v>165.1</v>
+        <v>25.4</v>
       </c>
       <c r="G221">
-        <v>165.1</v>
+        <v>101.6</v>
       </c>
       <c r="H221" t="s">
         <v>19</v>
+      </c>
+      <c r="I221" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="C222">
+        <v>50</v>
       </c>
       <c r="D222">
-        <v>0</v>
+        <v>9.9773242630385486</v>
+      </c>
+      <c r="E222">
+        <v>165.1</v>
+      </c>
+      <c r="F222">
+        <v>165.1</v>
+      </c>
+      <c r="G222">
+        <v>165.1</v>
+      </c>
+      <c r="H222" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
-        <v>240</v>
-      </c>
-      <c r="C223">
-        <v>1</v>
+        <v>239</v>
       </c>
       <c r="D223">
-        <v>2.2675736961451252</v>
-      </c>
-      <c r="E223">
-        <v>203.2</v>
-      </c>
-      <c r="F223">
-        <v>88.899999999999991</v>
-      </c>
-      <c r="G223">
-        <v>508</v>
-      </c>
-      <c r="H223" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
-        <v>241</v>
-      </c>
-      <c r="B224">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="C224">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D224">
-        <v>0</v>
+        <v>2.2675736961451252</v>
       </c>
       <c r="E224">
-        <v>76.199999999999989</v>
+        <v>203.2</v>
       </c>
       <c r="F224">
-        <v>38.099999999999987</v>
+        <v>88.899999999999991</v>
       </c>
       <c r="G224">
-        <v>3683</v>
+        <v>508</v>
       </c>
       <c r="H224" t="s">
         <v>19</v>
-      </c>
-      <c r="I224" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B225">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C225">
         <v>10</v>
@@ -6831,7 +7008,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G225">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H225" t="s">
         <v>19</v>
@@ -6842,7 +7019,10 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+      <c r="B226">
+        <v>289</v>
       </c>
       <c r="C226">
         <v>10</v>
@@ -6857,7 +7037,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G226">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H226" t="s">
         <v>19</v>
@@ -6868,25 +7048,22 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
-        <v>244</v>
-      </c>
-      <c r="B227">
-        <v>145</v>
+        <v>243</v>
       </c>
       <c r="C227">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D227">
         <v>0</v>
       </c>
       <c r="E227">
-        <v>57.15</v>
+        <v>76.199999999999989</v>
       </c>
       <c r="F227">
         <v>38.099999999999987</v>
       </c>
       <c r="G227">
-        <v>3683</v>
+        <v>1828.8</v>
       </c>
       <c r="H227" t="s">
         <v>19</v>
@@ -6897,10 +7074,10 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B228">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C228">
         <v>20</v>
@@ -6915,7 +7092,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G228">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H228" t="s">
         <v>19</v>
@@ -6926,25 +7103,25 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B229">
-        <v>145</v>
+        <v>289</v>
       </c>
       <c r="C229">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D229">
-        <v>10.612244897959179</v>
+        <v>0</v>
       </c>
       <c r="E229">
-        <v>76.199999999999989</v>
+        <v>57.15</v>
       </c>
       <c r="F229">
         <v>38.099999999999987</v>
       </c>
       <c r="G229">
-        <v>3683</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H229" t="s">
         <v>19</v>
@@ -6955,16 +7132,16 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B230">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C230">
         <v>10</v>
       </c>
       <c r="D230">
-        <v>21.22448979591837</v>
+        <v>10.612244897959179</v>
       </c>
       <c r="E230">
         <v>76.199999999999989</v>
@@ -6973,7 +7150,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G230">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H230" t="s">
         <v>19</v>
@@ -6984,13 +7161,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="B231">
+        <v>289</v>
       </c>
       <c r="C231">
         <v>10</v>
       </c>
       <c r="D231">
-        <v>5.3061224489795924</v>
+        <v>21.22448979591837</v>
       </c>
       <c r="E231">
         <v>76.199999999999989</v>
@@ -6999,7 +7179,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G231">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H231" t="s">
         <v>19</v>
@@ -7010,25 +7190,22 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
-        <v>249</v>
-      </c>
-      <c r="B232">
-        <v>145</v>
+        <v>248</v>
       </c>
       <c r="C232">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D232">
-        <v>9.7052154195011333</v>
+        <v>5.3061224489795924</v>
       </c>
       <c r="E232">
-        <v>57.15</v>
+        <v>76.199999999999989</v>
       </c>
       <c r="F232">
         <v>38.099999999999987</v>
       </c>
       <c r="G232">
-        <v>3683</v>
+        <v>1828.8</v>
       </c>
       <c r="H232" t="s">
         <v>19</v>
@@ -7039,16 +7216,16 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B233">
-        <v>289</v>
+        <v>145</v>
       </c>
       <c r="C233">
         <v>20</v>
       </c>
       <c r="D233">
-        <v>19.41043083900227</v>
+        <v>9.7052154195011333</v>
       </c>
       <c r="E233">
         <v>57.15</v>
@@ -7057,7 +7234,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G233">
-        <v>7340.5999999999995</v>
+        <v>3683</v>
       </c>
       <c r="H233" t="s">
         <v>19</v>
@@ -7068,13 +7245,16 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="B234">
+        <v>289</v>
       </c>
       <c r="C234">
         <v>20</v>
       </c>
       <c r="D234">
-        <v>4.8526077097505667</v>
+        <v>19.41043083900227</v>
       </c>
       <c r="E234">
         <v>57.15</v>
@@ -7083,7 +7263,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G234">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H234" t="s">
         <v>19</v>
@@ -7094,22 +7274,22 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C235">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D235">
-        <v>10.612244897959179</v>
+        <v>4.8526077097505667</v>
       </c>
       <c r="E235">
-        <v>76.199999999999989</v>
+        <v>57.15</v>
       </c>
       <c r="F235">
         <v>38.099999999999987</v>
       </c>
       <c r="G235">
-        <v>3683</v>
+        <v>1828.8</v>
       </c>
       <c r="H235" t="s">
         <v>19</v>
@@ -7120,19 +7300,19 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C236">
         <v>10</v>
       </c>
       <c r="D236">
-        <v>1.517857142857143</v>
+        <v>10.612244897959179</v>
       </c>
       <c r="E236">
-        <v>88.899999999999991</v>
+        <v>76.199999999999989</v>
       </c>
       <c r="F236">
-        <v>63.5</v>
+        <v>38.099999999999987</v>
       </c>
       <c r="G236">
         <v>3683</v>
@@ -7146,13 +7326,13 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C237">
         <v>10</v>
       </c>
       <c r="D237">
-        <v>0.75892857142857129</v>
+        <v>1.517857142857143</v>
       </c>
       <c r="E237">
         <v>88.899999999999991</v>
@@ -7161,7 +7341,7 @@
         <v>63.5</v>
       </c>
       <c r="G237">
-        <v>1828.8</v>
+        <v>3683</v>
       </c>
       <c r="H237" t="s">
         <v>19</v>
@@ -7172,76 +7352,82 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="C238">
+        <v>10</v>
       </c>
       <c r="D238">
-        <v>0</v>
+        <v>0.75892857142857129</v>
+      </c>
+      <c r="E238">
+        <v>88.899999999999991</v>
+      </c>
+      <c r="F238">
+        <v>63.5</v>
+      </c>
+      <c r="G238">
+        <v>1828.8</v>
+      </c>
+      <c r="H238" t="s">
+        <v>19</v>
+      </c>
+      <c r="I238" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
-        <v>256</v>
-      </c>
-      <c r="C239">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="D239">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E239">
-        <v>5</v>
-      </c>
-      <c r="F239">
-        <v>25.4</v>
-      </c>
-      <c r="G239">
-        <v>25</v>
-      </c>
-      <c r="H239" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C240">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D240">
-        <v>0.1004464285714286</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E240">
-        <v>76.199999999999989</v>
+        <v>5</v>
       </c>
       <c r="F240">
         <v>25.4</v>
       </c>
       <c r="G240">
-        <v>101.6</v>
+        <v>25</v>
       </c>
       <c r="H240" t="s">
         <v>19</v>
+      </c>
+      <c r="I240" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C241">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D241">
-        <v>2.410714285714286</v>
+        <v>0.1004464285714286</v>
       </c>
       <c r="E241">
-        <v>203.2</v>
+        <v>76.199999999999989</v>
       </c>
       <c r="F241">
+        <v>25.4</v>
+      </c>
+      <c r="G241">
         <v>101.6</v>
-      </c>
-      <c r="G241">
-        <v>459</v>
       </c>
       <c r="H241" t="s">
         <v>19</v>
@@ -7252,10 +7438,7 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
-        <v>259</v>
-      </c>
-      <c r="B242">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="C242">
         <v>10</v>
@@ -7281,7 +7464,10 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="B243">
+        <v>289</v>
       </c>
       <c r="C243">
         <v>10</v>
@@ -7307,7 +7493,7 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C244">
         <v>10</v>
@@ -7333,36 +7519,39 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C245">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D245">
-        <v>5.0000000000000001E-3</v>
+        <v>2.410714285714286</v>
       </c>
       <c r="E245">
-        <v>25.4</v>
+        <v>203.2</v>
       </c>
       <c r="F245">
-        <v>19.05</v>
+        <v>101.6</v>
       </c>
       <c r="G245">
-        <v>25.4</v>
+        <v>459</v>
       </c>
       <c r="H245" t="s">
         <v>19</v>
+      </c>
+      <c r="I245" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C246">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D246">
-        <v>0.29821428571428571</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E246">
         <v>25.4</v>
@@ -7376,42 +7565,48 @@
       <c r="H246" t="s">
         <v>19</v>
       </c>
+      <c r="I246" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
-        <v>264</v>
-      </c>
-      <c r="B247">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="C247">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D247">
-        <v>8.928571428571427</v>
+        <v>0.29821428571428571</v>
       </c>
       <c r="E247">
-        <v>63.5</v>
+        <v>25.4</v>
       </c>
       <c r="F247">
-        <v>38.099999999999987</v>
+        <v>19.05</v>
       </c>
       <c r="G247">
-        <v>7340.5999999999995</v>
+        <v>25.4</v>
       </c>
       <c r="H247" t="s">
         <v>19</v>
+      </c>
+      <c r="I247" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="B248">
+        <v>289</v>
       </c>
       <c r="C248">
         <v>1</v>
       </c>
       <c r="D248">
-        <v>2.2650450000000002</v>
+        <v>8.928571428571427</v>
       </c>
       <c r="E248">
         <v>63.5</v>
@@ -7420,7 +7615,7 @@
         <v>38.099999999999987</v>
       </c>
       <c r="G248">
-        <v>1828.8</v>
+        <v>7340.5999999999995</v>
       </c>
       <c r="H248" t="s">
         <v>19</v>
@@ -7428,22 +7623,22 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C249">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D249">
-        <v>10.793650793650791</v>
+        <v>2.2650450000000002</v>
       </c>
       <c r="E249">
-        <v>355.6</v>
+        <v>63.5</v>
       </c>
       <c r="F249">
-        <v>279.39999999999998</v>
+        <v>38.099999999999987</v>
       </c>
       <c r="G249">
-        <v>355.6</v>
+        <v>1828.8</v>
       </c>
       <c r="H249" t="s">
         <v>19</v>
@@ -7451,15 +7646,33 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+      <c r="C250">
+        <v>18</v>
       </c>
       <c r="D250">
-        <v>0</v>
+        <v>10.793650793650791</v>
+      </c>
+      <c r="E250">
+        <v>355.6</v>
+      </c>
+      <c r="F250">
+        <v>279.39999999999998</v>
+      </c>
+      <c r="G250">
+        <v>355.6</v>
+      </c>
+      <c r="H250" t="s">
+        <v>19</v>
+      </c>
+      <c r="I250" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -7467,7 +7680,7 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -7475,7 +7688,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -7483,7 +7696,7 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -7491,7 +7704,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -7499,7 +7712,7 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -7507,7 +7720,7 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -7515,7 +7728,7 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -7523,7 +7736,7 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -7531,7 +7744,7 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -7539,7 +7752,7 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -7547,7 +7760,7 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -7555,7 +7768,7 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -7563,7 +7776,7 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -7571,45 +7784,30 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
-        <v>282</v>
-      </c>
-      <c r="C265">
-        <v>100</v>
+        <v>281</v>
       </c>
       <c r="D265">
-        <v>0.26785714285714279</v>
-      </c>
-      <c r="E265">
-        <v>101.6</v>
-      </c>
-      <c r="F265">
-        <v>25.4</v>
-      </c>
-      <c r="G265">
-        <v>127</v>
-      </c>
-      <c r="H265" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C266">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D266">
-        <v>0.80357142857142849</v>
+        <v>0.26785714285714279</v>
       </c>
       <c r="E266">
+        <v>101.6</v>
+      </c>
+      <c r="F266">
+        <v>25.4</v>
+      </c>
+      <c r="G266">
         <v>127</v>
-      </c>
-      <c r="F266">
-        <v>50.8</v>
-      </c>
-      <c r="G266">
-        <v>177.8</v>
       </c>
       <c r="H266" t="s">
         <v>19</v>
@@ -7617,45 +7815,89 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
+        <v>283</v>
+      </c>
+      <c r="C267">
+        <v>10</v>
+      </c>
+      <c r="D267">
+        <v>0.80357142857142849</v>
+      </c>
+      <c r="E267">
+        <v>127</v>
+      </c>
+      <c r="F267">
+        <v>50.8</v>
+      </c>
+      <c r="G267">
+        <v>177.8</v>
+      </c>
+      <c r="H267" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A268" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D267">
+      <c r="B268" s="3"/>
+      <c r="C268" s="3"/>
+      <c r="D268" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A268" t="s">
-        <v>285</v>
-      </c>
-      <c r="D268">
-        <v>0</v>
-      </c>
+      <c r="E268" s="3"/>
+      <c r="F268" s="3"/>
+      <c r="G268" s="3"/>
+      <c r="H268" s="3"/>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D269">
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A270" t="s">
-        <v>287</v>
-      </c>
-      <c r="D270">
+      <c r="A270" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B270" s="3"/>
+      <c r="C270" s="3"/>
+      <c r="D270" s="3">
         <v>0</v>
       </c>
+      <c r="E270" s="3"/>
+      <c r="F270" s="3"/>
+      <c r="G270" s="3"/>
+      <c r="H270" s="3"/>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D271">
         <v>0</v>
       </c>
     </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A272" t="s">
+        <v>287</v>
+      </c>
+      <c r="D272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A273" t="s">
+        <v>288</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Hotfix for output decimal places
</commit_message>
<xml_diff>
--- a/src/Sub-Bundle_Data.xlsx
+++ b/src/Sub-Bundle_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\Optimizer\Optimizer SW 251202\_internal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5BDE06-14A4-4A41-8D1A-B85A2613EF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232C4C1-BECB-4CE7-88AC-9A8C8FC0D6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="10650" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2505" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Bundle_Data" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1400,23 +1401,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="L247" sqref="L247"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>90</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>92</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>95</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>97</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>98</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>99</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>105</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>106</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>108</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>109</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>110</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>111</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>113</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>118</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>119</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>120</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>122</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>123</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>124</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>125</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>126</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>127</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>128</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>130</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>132</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>133</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>134</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>136</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>137</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>139</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>140</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>144</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>145</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>147</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>148</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>151</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>152</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>153</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>154</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>155</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>156</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>157</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>158</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>159</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>160</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>162</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>165</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>166</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>167</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>168</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>169</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>170</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>171</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>172</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>173</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>174</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>175</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>176</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>177</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>178</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>179</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>180</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>181</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>182</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>183</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>184</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>185</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>186</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>187</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>188</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>189</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>325</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
         <v>190</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>191</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>192</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>193</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>195</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>196</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>197</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>198</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>199</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>200</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>201</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>202</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>203</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>204</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>205</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>206</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>207</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>208</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>209</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>210</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>211</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>212</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>213</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>214</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>215</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>216</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>217</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>219</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>220</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>221</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>222</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>223</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>224</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>225</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>226</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>227</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>228</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>229</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>230</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>231</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>232</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>233</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>234</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>235</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>236</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>237</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>238</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>239</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>240</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>241</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>242</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>243</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>244</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>245</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>246</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>247</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>248</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>249</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>250</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>251</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>252</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>253</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>254</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>255</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>256</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>257</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>258</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>259</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>260</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>261</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>262</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>263</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>264</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>265</v>
       </c>
@@ -7644,7 +7644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>266</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>267</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>268</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>269</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>270</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>271</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>272</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>273</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>274</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>275</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>276</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>277</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>278</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>279</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>280</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>281</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>282</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>283</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" s="3" t="s">
         <v>284</v>
       </c>
@@ -7850,7 +7850,7 @@
       <c r="G268" s="3"/>
       <c r="H268" s="3"/>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>285</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" s="3" t="s">
         <v>326</v>
       </c>
@@ -7872,7 +7872,7 @@
       <c r="G270" s="3"/>
       <c r="H270" s="3"/>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>286</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>287</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>288</v>
       </c>
@@ -7908,184 +7908,184 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>324</v>
       </c>

</xml_diff>